<commit_message>
First Trials using 500.000 images
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -1,361 +1,487 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="logs" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="logs" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="112">
-  <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Network</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validation size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rand seed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shuffler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optimizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loss function</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr_init</t>
-  </si>
-  <si>
-    <t xml:space="preserve">momentum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr scheduler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr decay period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pretrained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of iter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loss_tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">loss_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCR_tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCR_test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rmse_tr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rmse_test</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="156">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Validation size</t>
+  </si>
+  <si>
+    <t>rand seed</t>
+  </si>
+  <si>
+    <t>shuffler</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>Loss function</t>
+  </si>
+  <si>
+    <t>lr_init</t>
+  </si>
+  <si>
+    <t>momentum</t>
+  </si>
+  <si>
+    <t>lr scheduler</t>
+  </si>
+  <si>
+    <t>lr decay period</t>
+  </si>
+  <si>
+    <t>pretrained</t>
+  </si>
+  <si>
+    <t>batch_size</t>
+  </si>
+  <si>
+    <t>Number of iter</t>
+  </si>
+  <si>
+    <t>loss_tr</t>
+  </si>
+  <si>
+    <t>loss_test</t>
+  </si>
+  <si>
+    <t>CCR_tr</t>
+  </si>
+  <si>
+    <t>CCR_test</t>
+  </si>
+  <si>
+    <t>rmse_tr</t>
+  </si>
+  <si>
+    <t>rmse_test</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">September04  23:43:02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resnet34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">True</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sgd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">crossentropy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f21bae489d8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September04  23:50:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f0fe21de950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September04  23:50:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September04  23:51:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f9d2a29f950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September04  23:55:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f9bcf3a7950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  00:47:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resnet18_real_sgd_multisoft_August29  19:06:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f9bcf3a78c8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  01:37:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resnet18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f03de734950&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  13:43:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f41d161f9d8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  13:44:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  14:10:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  14:37:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  15:07:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  15:33:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  16:00:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  16:27:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  16:53:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  17:20:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  17:45:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  18:13:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  18:42:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  19:10:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  19:38:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  20:06:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  20:34:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  21:38:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  22:07:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  22:35:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  23:03:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  23:30:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September05  23:58:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September06  00:25:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:28:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multisoft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;function exp_lr_scheduler at 0x7f42d652c9d8&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:29:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:30:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:32:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:43:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:49:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  18:59:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  21:14:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  21:42:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  22:10:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  22:38:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  23:05:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September07  23:33:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  00:02:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  00:30:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  00:58:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  01:26:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  01:54:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  02:22:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  02:50:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  03:18:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  03:46:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  04:13:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  04:40:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  05:08:18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  05:36:37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  06:04:39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  06:32:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  06:59:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">September08  07:27:10</t>
+    <t>September04  23:43:02</t>
+  </si>
+  <si>
+    <t>resnet34</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>sgd</t>
+  </si>
+  <si>
+    <t>crossentropy</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f21bae489d8&gt;</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>September04  23:50:13</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f0fe21de950&gt;</t>
+  </si>
+  <si>
+    <t>September04  23:50:54</t>
+  </si>
+  <si>
+    <t>September04  23:51:36</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f9d2a29f950&gt;</t>
+  </si>
+  <si>
+    <t>September04  23:55:12</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f9bcf3a7950&gt;</t>
+  </si>
+  <si>
+    <t>September05  00:47:46</t>
+  </si>
+  <si>
+    <t>resnet18_real_sgd_multisoft_August29  19:06:27</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f9bcf3a78c8&gt;</t>
+  </si>
+  <si>
+    <t>September05  01:37:16</t>
+  </si>
+  <si>
+    <t>resnet18</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f03de734950&gt;</t>
+  </si>
+  <si>
+    <t>September05  13:43:58</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f41d161f9d8&gt;</t>
+  </si>
+  <si>
+    <t>September05  13:44:42</t>
+  </si>
+  <si>
+    <t>September05  14:10:59</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>September05  14:37:45</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>September05  15:07:00</t>
+  </si>
+  <si>
+    <t>September05  15:33:27</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>September05  16:00:39</t>
+  </si>
+  <si>
+    <t>0.03</t>
+  </si>
+  <si>
+    <t>September05  16:27:07</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>September05  16:53:37</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>September05  17:20:06</t>
+  </si>
+  <si>
+    <t>September05  17:45:51</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>September05  18:13:45</t>
+  </si>
+  <si>
+    <t>0.005</t>
+  </si>
+  <si>
+    <t>September05  18:42:09</t>
+  </si>
+  <si>
+    <t>September05  19:10:48</t>
+  </si>
+  <si>
+    <t>September05  19:38:54</t>
+  </si>
+  <si>
+    <t>September05  20:06:39</t>
+  </si>
+  <si>
+    <t>September05  20:34:09</t>
+  </si>
+  <si>
+    <t>September05  21:38:53</t>
+  </si>
+  <si>
+    <t>September05  22:07:23</t>
+  </si>
+  <si>
+    <t>September05  22:35:24</t>
+  </si>
+  <si>
+    <t>September05  23:03:10</t>
+  </si>
+  <si>
+    <t>September05  23:30:51</t>
+  </si>
+  <si>
+    <t>September05  23:58:24</t>
+  </si>
+  <si>
+    <t>September06  00:25:51</t>
+  </si>
+  <si>
+    <t>September07  18:28:27</t>
+  </si>
+  <si>
+    <t>multisoft</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f42d652c9d8&gt;</t>
+  </si>
+  <si>
+    <t>September07  18:29:26</t>
+  </si>
+  <si>
+    <t>September07  18:30:03</t>
+  </si>
+  <si>
+    <t>September07  18:32:20</t>
+  </si>
+  <si>
+    <t>September07  18:43:30</t>
+  </si>
+  <si>
+    <t>September07  18:49:22</t>
+  </si>
+  <si>
+    <t>September07  18:59:28</t>
+  </si>
+  <si>
+    <t>September07  21:14:30</t>
+  </si>
+  <si>
+    <t>September07  21:42:06</t>
+  </si>
+  <si>
+    <t>September07  22:10:09</t>
+  </si>
+  <si>
+    <t>September07  22:38:05</t>
+  </si>
+  <si>
+    <t>September07  23:05:54</t>
+  </si>
+  <si>
+    <t>September07  23:33:58</t>
+  </si>
+  <si>
+    <t>September08  00:02:13</t>
+  </si>
+  <si>
+    <t>September08  00:30:31</t>
+  </si>
+  <si>
+    <t>September08  00:58:30</t>
+  </si>
+  <si>
+    <t>September08  01:26:34</t>
+  </si>
+  <si>
+    <t>September08  01:54:36</t>
+  </si>
+  <si>
+    <t>September08  02:22:39</t>
+  </si>
+  <si>
+    <t>September08  02:50:38</t>
+  </si>
+  <si>
+    <t>September08  03:18:37</t>
+  </si>
+  <si>
+    <t>September08  03:46:14</t>
+  </si>
+  <si>
+    <t>September08  04:13:36</t>
+  </si>
+  <si>
+    <t>September08  04:40:54</t>
+  </si>
+  <si>
+    <t>September08  05:08:18</t>
+  </si>
+  <si>
+    <t>September08  05:36:37</t>
+  </si>
+  <si>
+    <t>September08  06:04:39</t>
+  </si>
+  <si>
+    <t>September08  06:32:26</t>
+  </si>
+  <si>
+    <t>September08  06:59:49</t>
+  </si>
+  <si>
+    <t>September08  07:27:10</t>
+  </si>
+  <si>
+    <t>September08  19:25:15</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f07136878c8&gt;</t>
+  </si>
+  <si>
+    <t>September08  19:39:30</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fbfef9a18c8&gt;</t>
+  </si>
+  <si>
+    <t>September08  20:05:57</t>
+  </si>
+  <si>
+    <t>September08  20:31:33</t>
+  </si>
+  <si>
+    <t>September08  20:57:15</t>
+  </si>
+  <si>
+    <t>September08  21:23:26</t>
+  </si>
+  <si>
+    <t>September08  21:49:10</t>
+  </si>
+  <si>
+    <t>September08  22:14:54</t>
+  </si>
+  <si>
+    <t>September08  22:40:37</t>
+  </si>
+  <si>
+    <t>September08  23:06:17</t>
+  </si>
+  <si>
+    <t>1.0xcross + 0.3Xmulti</t>
+  </si>
+  <si>
+    <t>September08  23:34:14</t>
+  </si>
+  <si>
+    <t>1.0xcross + 0.6Xmulti</t>
+  </si>
+  <si>
+    <t>September09  00:02:21</t>
+  </si>
+  <si>
+    <t>1.0xcross + 1.0Xmulti</t>
+  </si>
+  <si>
+    <t>September09  00:30:24</t>
+  </si>
+  <si>
+    <t>1.0xcross + 1.5Xmulti</t>
+  </si>
+  <si>
+    <t>September09  00:58:26</t>
+  </si>
+  <si>
+    <t>1.0xcross + 2.0Xmulti</t>
+  </si>
+  <si>
+    <t>September09  01:26:33</t>
+  </si>
+  <si>
+    <t>1.0xcross + 5.0Xmulti</t>
+  </si>
+  <si>
+    <t>September09  01:54:42</t>
+  </si>
+  <si>
+    <t>1.0xcross + 10.0Xmulti</t>
+  </si>
+  <si>
+    <t>September09  02:22:47</t>
+  </si>
+  <si>
+    <t>September09  02:50:49</t>
+  </si>
+  <si>
+    <t>September09  03:18:55</t>
+  </si>
+  <si>
+    <t>September09  03:46:53</t>
+  </si>
+  <si>
+    <t>September09  04:14:49</t>
+  </si>
+  <si>
+    <t>September09  04:42:52</t>
+  </si>
+  <si>
+    <t>September09  05:10:44</t>
+  </si>
+  <si>
+    <t>September09  05:38:27</t>
+  </si>
+  <si>
+    <t>September09  06:05:48</t>
+  </si>
+  <si>
+    <t>September09  06:33:03</t>
+  </si>
+  <si>
+    <t>September09  07:00:11</t>
+  </si>
+  <si>
+    <t>September09  07:27:46</t>
+  </si>
+  <si>
+    <t>September09  07:55:06</t>
+  </si>
+  <si>
+    <t>September09  08:22:15</t>
+  </si>
+  <si>
+    <t>September11  09:15:15</t>
+  </si>
+  <si>
+    <t>1.0xcross + 0.0Xmulti</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7ff8b6f8e8c8&gt;</t>
+  </si>
+  <si>
+    <t>64</t>
   </si>
 </sst>
 </file>
@@ -363,48 +489,48 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt formatCode="General" numFmtId="164"/>
   </numFmts>
   <fonts count="5">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -412,78 +538,344 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:T64"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="65:65"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A41" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A72" activeCellId="0" pane="topLeft" sqref="66:72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.1224489795918"/>
+    <col customWidth="1" max="1" min="1" style="1" width="9.719387755102041"/>
+    <col customWidth="1" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col customWidth="1" max="4" min="3" style="1" width="9.719387755102041"/>
+    <col customWidth="1" max="5" min="5" style="1" width="13.7704081632653"/>
+    <col customWidth="1" max="6" min="6" style="1" width="10.6632653061225"/>
+    <col customWidth="1" max="1025" min="7" style="1" width="9.719387755102041"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="13.8" r="1" s="3" spans="1:20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -545,54 +937,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
-      <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
+    <row customHeight="1" ht="12.8" r="2" s="3" spans="1:20">
       <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="0"/>
-      <c r="T2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
-      <c r="Q3" s="0"/>
+      <c r="R2" s="1" t="n"/>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="3" spans="1:20">
       <c r="R3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="0"/>
-      <c r="T3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="4" s="3" spans="1:20">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -647,10 +1003,8 @@
       <c r="R4" s="1" t="n">
         <v>0.732</v>
       </c>
-      <c r="S4" s="0"/>
-      <c r="T4" s="0"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="5" s="3" spans="1:20">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -690,12 +1044,16 @@
       <c r="M5" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="N5" s="1" t="n"/>
+      <c r="O5" s="1" t="n"/>
+      <c r="P5" s="1" t="n"/>
+      <c r="Q5" s="1" t="n"/>
+      <c r="R5" s="1" t="n"/>
       <c r="S5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="6" s="3" spans="1:20">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -735,12 +1093,16 @@
       <c r="M6" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="N6" s="1" t="n"/>
+      <c r="O6" s="1" t="n"/>
+      <c r="P6" s="1" t="n"/>
+      <c r="Q6" s="1" t="n"/>
+      <c r="R6" s="1" t="n"/>
       <c r="S6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="7" s="3" spans="1:20">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -780,12 +1142,16 @@
       <c r="M7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="N7" s="1" t="n"/>
+      <c r="O7" s="1" t="n"/>
+      <c r="P7" s="1" t="n"/>
+      <c r="Q7" s="1" t="n"/>
+      <c r="R7" s="1" t="n"/>
       <c r="S7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="8" s="3" spans="1:20">
       <c r="A8" s="1" t="s">
         <v>38</v>
       </c>
@@ -835,7 +1201,7 @@
         <v>0.0426815513372421</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <v>0.53052776819593</v>
+        <v>0.5305277681959299</v>
       </c>
       <c r="R8" s="1" t="n">
         <v>0.419</v>
@@ -843,9 +1209,8 @@
       <c r="S8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="9" s="3" spans="1:20">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
@@ -903,9 +1268,8 @@
       <c r="S9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="10" s="3" spans="1:20">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
@@ -963,9 +1327,8 @@
       <c r="S10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="11" s="3" spans="1:20">
       <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
@@ -1005,17 +1368,11 @@
       <c r="M11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="0"/>
-      <c r="O11" s="0"/>
-      <c r="P11" s="0"/>
-      <c r="Q11" s="0"/>
-      <c r="R11" s="0"/>
       <c r="S11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="12" s="3" spans="1:20">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -1073,9 +1430,8 @@
       <c r="S12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="13" s="3" spans="1:20">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1133,9 +1489,8 @@
       <c r="S13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="14" s="3" spans="1:20">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1193,9 +1548,8 @@
       <c r="S14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="15" s="3" spans="1:20">
       <c r="A15" s="1" t="s">
         <v>54</v>
       </c>
@@ -1253,9 +1607,8 @@
       <c r="S15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="16" s="3" spans="1:20">
       <c r="A16" s="1" t="s">
         <v>55</v>
       </c>
@@ -1313,9 +1666,8 @@
       <c r="S16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="17" s="3" spans="1:20">
       <c r="A17" s="1" t="s">
         <v>57</v>
       </c>
@@ -1373,9 +1725,8 @@
       <c r="S17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="18" s="3" spans="1:20">
       <c r="A18" s="1" t="s">
         <v>59</v>
       </c>
@@ -1433,9 +1784,8 @@
       <c r="S18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="19" s="3" spans="1:20">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -1493,9 +1843,8 @@
       <c r="S19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T19" s="0"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="20" s="3" spans="1:20">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1553,9 +1902,8 @@
       <c r="S20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="21" s="3" spans="1:20">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -1613,9 +1961,8 @@
       <c r="S21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="22" s="3" spans="1:20">
       <c r="A22" s="1" t="s">
         <v>66</v>
       </c>
@@ -1673,9 +2020,8 @@
       <c r="S22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="23" s="3" spans="1:20">
       <c r="A23" s="1" t="s">
         <v>68</v>
       </c>
@@ -1733,9 +2079,8 @@
       <c r="S23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="24" s="3" spans="1:20">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -1793,9 +2138,8 @@
       <c r="S24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="25" s="3" spans="1:20">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
@@ -1853,9 +2197,8 @@
       <c r="S25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="26" s="3" spans="1:20">
       <c r="A26" s="1" t="s">
         <v>71</v>
       </c>
@@ -1913,9 +2256,8 @@
       <c r="S26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="27" s="3" spans="1:20">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -1973,9 +2315,8 @@
       <c r="S27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="28" s="3" spans="1:20">
       <c r="A28" s="1" t="s">
         <v>73</v>
       </c>
@@ -2033,9 +2374,8 @@
       <c r="S28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="29" s="3" spans="1:20">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -2093,9 +2433,8 @@
       <c r="S29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="30" s="3" spans="1:20">
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
@@ -2153,9 +2492,8 @@
       <c r="S30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="31" s="3" spans="1:20">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -2213,9 +2551,8 @@
       <c r="S31" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="32" s="3" spans="1:20">
       <c r="A32" s="1" t="s">
         <v>77</v>
       </c>
@@ -2273,9 +2610,8 @@
       <c r="S32" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="33" s="3" spans="1:20">
       <c r="A33" s="1" t="s">
         <v>78</v>
       </c>
@@ -2333,9 +2669,8 @@
       <c r="S33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="34" s="3" spans="1:20">
       <c r="A34" s="1" t="s">
         <v>79</v>
       </c>
@@ -2393,9 +2728,8 @@
       <c r="S34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="35" s="3" spans="1:20">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2435,17 +2769,11 @@
       <c r="M35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N35" s="0"/>
-      <c r="O35" s="0"/>
-      <c r="P35" s="0"/>
-      <c r="Q35" s="0"/>
-      <c r="R35" s="0"/>
       <c r="S35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="36" s="3" spans="1:20">
       <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
@@ -2485,17 +2813,11 @@
       <c r="M36" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N36" s="0"/>
-      <c r="O36" s="0"/>
-      <c r="P36" s="0"/>
-      <c r="Q36" s="0"/>
-      <c r="R36" s="0"/>
       <c r="S36" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="37" s="3" spans="1:20">
       <c r="A37" s="1" t="s">
         <v>84</v>
       </c>
@@ -2535,17 +2857,11 @@
       <c r="M37" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N37" s="0"/>
-      <c r="O37" s="0"/>
-      <c r="P37" s="0"/>
-      <c r="Q37" s="0"/>
-      <c r="R37" s="0"/>
       <c r="S37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="38" s="3" spans="1:20">
       <c r="A38" s="1" t="s">
         <v>85</v>
       </c>
@@ -2607,7 +2923,7 @@
         <v>1.20457461371224</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="39" s="3" spans="1:20">
       <c r="A39" s="1" t="s">
         <v>86</v>
       </c>
@@ -2647,17 +2963,11 @@
       <c r="M39" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N39" s="0"/>
-      <c r="O39" s="0"/>
-      <c r="P39" s="0"/>
-      <c r="Q39" s="0"/>
-      <c r="R39" s="0"/>
       <c r="S39" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="T39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row customHeight="1" ht="12.8" r="40" s="3" spans="1:20">
       <c r="A40" s="1" t="s">
         <v>87</v>
       </c>
@@ -2719,7 +3029,7 @@
         <v>1.05830052442584</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="41" s="3" spans="1:20">
       <c r="A41" s="1" t="s">
         <v>88</v>
       </c>
@@ -2781,7 +3091,7 @@
         <v>1.06723942955646</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="42" s="3" spans="1:20">
       <c r="A42" s="1" t="s">
         <v>89</v>
       </c>
@@ -2825,7 +3135,7 @@
         <v>12</v>
       </c>
       <c r="O42" s="1" t="n">
-        <v>0.00809854276480861</v>
+        <v>0.008098542764808611</v>
       </c>
       <c r="P42" s="1" t="n">
         <v>0.0160511491298676</v>
@@ -2843,7 +3153,7 @@
         <v>1.03440804327886</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="43" s="3" spans="1:20">
       <c r="A43" s="1" t="s">
         <v>90</v>
       </c>
@@ -2905,7 +3215,7 @@
         <v>1.04737767782209</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="44" s="3" spans="1:20">
       <c r="A44" s="1" t="s">
         <v>91</v>
       </c>
@@ -2967,7 +3277,7 @@
         <v>1.04928547116597</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="45" s="3" spans="1:20">
       <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
@@ -3029,7 +3339,7 @@
         <v>1.06677082824757</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="46" s="3" spans="1:20">
       <c r="A46" s="1" t="s">
         <v>93</v>
       </c>
@@ -3091,7 +3401,7 @@
         <v>1.09954536059228</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="47" s="3" spans="1:20">
       <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
@@ -3153,7 +3463,7 @@
         <v>1.06395488626163</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="48" s="3" spans="1:20">
       <c r="A48" s="1" t="s">
         <v>95</v>
       </c>
@@ -3215,7 +3525,7 @@
         <v>1.04355162785557</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="49" s="3" spans="1:20">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -3277,7 +3587,7 @@
         <v>1.0397114984456</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="50" s="3" spans="1:20">
       <c r="A50" s="1" t="s">
         <v>97</v>
       </c>
@@ -3339,7 +3649,7 @@
         <v>1.03537432844358</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="51" s="3" spans="1:20">
       <c r="A51" s="1" t="s">
         <v>98</v>
       </c>
@@ -3401,7 +3711,7 @@
         <v>1.08949529599719</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="52" s="3" spans="1:20">
       <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
@@ -3463,7 +3773,7 @@
         <v>1.06630202100531</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="53" s="3" spans="1:20">
       <c r="A53" s="1" t="s">
         <v>100</v>
       </c>
@@ -3513,7 +3823,7 @@
         <v>0.0564729008674622</v>
       </c>
       <c r="Q53" s="1" t="n">
-        <v>0.695929630907209</v>
+        <v>0.6959296309072091</v>
       </c>
       <c r="R53" s="1" t="n">
         <v>0.355</v>
@@ -3525,7 +3835,7 @@
         <v>1.15628716156498</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="54" s="3" spans="1:20">
       <c r="A54" s="1" t="s">
         <v>101</v>
       </c>
@@ -3587,7 +3897,7 @@
         <v>1.09453186340097</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="55" s="3" spans="1:20">
       <c r="A55" s="1" t="s">
         <v>102</v>
       </c>
@@ -3649,7 +3959,7 @@
         <v>1.17430830704717</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="56" s="3" spans="1:20">
       <c r="A56" s="1" t="s">
         <v>103</v>
       </c>
@@ -3711,7 +4021,7 @@
         <v>1.21119775429118</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="57" s="3" spans="1:20">
       <c r="A57" s="1" t="s">
         <v>104</v>
       </c>
@@ -3773,7 +4083,7 @@
         <v>1.1933147112141</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="58" s="3" spans="1:20">
       <c r="A58" s="1" t="s">
         <v>105</v>
       </c>
@@ -3835,7 +4145,7 @@
         <v>1.20249740124459</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="59" s="3" spans="1:20">
       <c r="A59" s="1" t="s">
         <v>106</v>
       </c>
@@ -3897,7 +4207,7 @@
         <v>1.10589330407594</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="60" s="3" spans="1:20">
       <c r="A60" s="1" t="s">
         <v>107</v>
       </c>
@@ -3959,7 +4269,7 @@
         <v>1.09635760589326</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="61" s="3" spans="1:20">
       <c r="A61" s="1" t="s">
         <v>108</v>
       </c>
@@ -4021,7 +4331,7 @@
         <v>1.16318528188763</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="62" s="3" spans="1:20">
       <c r="A62" s="1" t="s">
         <v>109</v>
       </c>
@@ -4083,7 +4393,7 @@
         <v>1.18490505948789</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="63" s="3" spans="1:20">
       <c r="A63" s="1" t="s">
         <v>110</v>
       </c>
@@ -4145,7 +4455,7 @@
         <v>1.18827606220104</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row customHeight="1" ht="12.8" r="64" s="3" spans="1:20">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
@@ -4207,13 +4517,1939 @@
         <v>1.21614143914267</v>
       </c>
     </row>
+    <row customHeight="1" ht="12.8" r="65" s="3" spans="1:20">
+      <c r="A65" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M65" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O65" s="1" t="n">
+        <v>0.00664125044038889</v>
+      </c>
+      <c r="P65" s="1" t="n">
+        <v>0.0064219431579113</v>
+      </c>
+      <c r="Q65" s="1" t="n">
+        <v>0.30027595722663</v>
+      </c>
+      <c r="R65" s="1" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="S65" s="1" t="n">
+        <v>1.19386727718926</v>
+      </c>
+      <c r="T65" s="1" t="n">
+        <v>1.17175082675456</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" t="s">
+        <v>23</v>
+      </c>
+      <c r="D66" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66" t="s">
+        <v>113</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
+      </c>
+      <c r="I66" t="s">
+        <v>29</v>
+      </c>
+      <c r="J66" t="s">
+        <v>116</v>
+      </c>
+      <c r="K66" t="s">
+        <v>31</v>
+      </c>
+      <c r="L66" t="s">
+        <v>25</v>
+      </c>
+      <c r="M66" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" t="n">
+        <v>25</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0.006075148203735641</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0.006006932407617569</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0.3009658502932046</v>
+      </c>
+      <c r="R66" t="n">
+        <v>0.341</v>
+      </c>
+      <c r="S66" t="n">
+        <v>1.140976869452849</v>
+      </c>
+      <c r="T66" t="n">
+        <v>1.120714058089752</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" t="s">
+        <v>117</v>
+      </c>
+      <c r="B67" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" t="s">
+        <v>56</v>
+      </c>
+      <c r="G67" t="s">
+        <v>113</v>
+      </c>
+      <c r="H67" t="s">
+        <v>58</v>
+      </c>
+      <c r="I67" t="s">
+        <v>29</v>
+      </c>
+      <c r="J67" t="s">
+        <v>116</v>
+      </c>
+      <c r="K67" t="s">
+        <v>31</v>
+      </c>
+      <c r="L67" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" t="s">
+        <v>32</v>
+      </c>
+      <c r="N67" t="n">
+        <v>30</v>
+      </c>
+      <c r="O67" t="n">
+        <v>0.006307549459815396</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0.006152551405131817</v>
+      </c>
+      <c r="Q67" t="n">
+        <v>0.3044153156260779</v>
+      </c>
+      <c r="R67" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="S67" t="n">
+        <v>1.163578593457619</v>
+      </c>
+      <c r="T67" t="n">
+        <v>1.136221809331259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" t="s">
+        <v>25</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68" t="s">
+        <v>113</v>
+      </c>
+      <c r="H68" t="s">
+        <v>60</v>
+      </c>
+      <c r="I68" t="s">
+        <v>29</v>
+      </c>
+      <c r="J68" t="s">
+        <v>116</v>
+      </c>
+      <c r="K68" t="s">
+        <v>31</v>
+      </c>
+      <c r="L68" t="s">
+        <v>25</v>
+      </c>
+      <c r="M68" t="s">
+        <v>32</v>
+      </c>
+      <c r="N68" t="n">
+        <v>28</v>
+      </c>
+      <c r="O68" t="n">
+        <v>0.006355568037984206</v>
+      </c>
+      <c r="P68" t="n">
+        <v>0.006062514111399651</v>
+      </c>
+      <c r="Q68" t="n">
+        <v>0.3026905829596412</v>
+      </c>
+      <c r="R68" t="n">
+        <v>0.307</v>
+      </c>
+      <c r="S68" t="n">
+        <v>1.164023188236675</v>
+      </c>
+      <c r="T68" t="n">
+        <v>1.127386357909302</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" t="s">
+        <v>119</v>
+      </c>
+      <c r="B69" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69" t="s">
+        <v>113</v>
+      </c>
+      <c r="H69" t="s">
+        <v>47</v>
+      </c>
+      <c r="I69" t="s">
+        <v>29</v>
+      </c>
+      <c r="J69" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69" t="s">
+        <v>31</v>
+      </c>
+      <c r="L69" t="s">
+        <v>25</v>
+      </c>
+      <c r="M69" t="s">
+        <v>32</v>
+      </c>
+      <c r="N69" t="n">
+        <v>25</v>
+      </c>
+      <c r="O69" t="n">
+        <v>0.006403026911524831</v>
+      </c>
+      <c r="P69" t="n">
+        <v>0.006266463056206703</v>
+      </c>
+      <c r="Q69" t="n">
+        <v>0.3025181096929976</v>
+      </c>
+      <c r="R69" t="n">
+        <v>0.297</v>
+      </c>
+      <c r="S69" t="n">
+        <v>1.172438456871</v>
+      </c>
+      <c r="T69" t="n">
+        <v>1.132254388377453</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" t="s">
+        <v>120</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" t="s">
+        <v>23</v>
+      </c>
+      <c r="D70" t="s">
+        <v>24</v>
+      </c>
+      <c r="E70" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" t="s">
+        <v>113</v>
+      </c>
+      <c r="H70" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" t="s">
+        <v>29</v>
+      </c>
+      <c r="J70" t="s">
+        <v>116</v>
+      </c>
+      <c r="K70" t="s">
+        <v>31</v>
+      </c>
+      <c r="L70" t="s">
+        <v>25</v>
+      </c>
+      <c r="M70" t="s">
+        <v>32</v>
+      </c>
+      <c r="N70" t="n">
+        <v>1</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0.02824255854929674</v>
+      </c>
+      <c r="P70" t="n">
+        <v>0.0284850013256073</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0.1710934805105209</v>
+      </c>
+      <c r="R70" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="S70" t="n">
+        <v>2.366184097188303</v>
+      </c>
+      <c r="T70" t="n">
+        <v>2.36093201935168</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" t="s">
+        <v>121</v>
+      </c>
+      <c r="B71" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" t="s">
+        <v>25</v>
+      </c>
+      <c r="F71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" t="s">
+        <v>113</v>
+      </c>
+      <c r="H71" t="s">
+        <v>58</v>
+      </c>
+      <c r="I71" t="s">
+        <v>29</v>
+      </c>
+      <c r="J71" t="s">
+        <v>116</v>
+      </c>
+      <c r="K71" t="s">
+        <v>31</v>
+      </c>
+      <c r="L71" t="s">
+        <v>25</v>
+      </c>
+      <c r="M71" t="s">
+        <v>32</v>
+      </c>
+      <c r="N71" t="n">
+        <v>1</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0.02822214595282148</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0.02824500125646591</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0.1657468092445671</v>
+      </c>
+      <c r="R71" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="S71" t="n">
+        <v>2.374152233362846</v>
+      </c>
+      <c r="T71" t="n">
+        <v>2.36093201935168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="A72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" t="s">
+        <v>24</v>
+      </c>
+      <c r="E72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" t="s">
+        <v>26</v>
+      </c>
+      <c r="G72" t="s">
+        <v>113</v>
+      </c>
+      <c r="H72" t="s">
+        <v>60</v>
+      </c>
+      <c r="I72" t="s">
+        <v>29</v>
+      </c>
+      <c r="J72" t="s">
+        <v>116</v>
+      </c>
+      <c r="K72" t="s">
+        <v>31</v>
+      </c>
+      <c r="L72" t="s">
+        <v>25</v>
+      </c>
+      <c r="M72" t="s">
+        <v>32</v>
+      </c>
+      <c r="N72" t="n">
+        <v>1</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0.02793271938308678</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0.02853000104427338</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0.1721283201103829</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="S72" t="n">
+        <v>2.362719243045114</v>
+      </c>
+      <c r="T72" t="n">
+        <v>2.36093201935168</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="A73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" t="s">
+        <v>113</v>
+      </c>
+      <c r="H73" t="s">
+        <v>47</v>
+      </c>
+      <c r="I73" t="s">
+        <v>29</v>
+      </c>
+      <c r="J73" t="s">
+        <v>116</v>
+      </c>
+      <c r="K73" t="s">
+        <v>31</v>
+      </c>
+      <c r="L73" t="s">
+        <v>25</v>
+      </c>
+      <c r="M73" t="s">
+        <v>32</v>
+      </c>
+      <c r="N73" t="n">
+        <v>1</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0.05550669897482616</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0.05739000225067139</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.02759572266298724</v>
+      </c>
+      <c r="R73" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="S73" t="n">
+        <v>3.324467916302756</v>
+      </c>
+      <c r="T73" t="n">
+        <v>3.348731102970198</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20">
+      <c r="A74" t="s">
+        <v>124</v>
+      </c>
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" t="s">
+        <v>125</v>
+      </c>
+      <c r="H74" t="s">
+        <v>67</v>
+      </c>
+      <c r="I74" t="s">
+        <v>29</v>
+      </c>
+      <c r="J74" t="s">
+        <v>116</v>
+      </c>
+      <c r="K74" t="s">
+        <v>31</v>
+      </c>
+      <c r="L74" t="s">
+        <v>25</v>
+      </c>
+      <c r="M74" t="s">
+        <v>32</v>
+      </c>
+      <c r="N74" t="n">
+        <v>9</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0.04140179559830017</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0.0503474736213684</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0.4813728872024836</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="S74" t="n">
+        <v>1.061411973607069</v>
+      </c>
+      <c r="T74" t="n">
+        <v>1.097269337947616</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20">
+      <c r="A75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" t="s">
+        <v>127</v>
+      </c>
+      <c r="H75" t="s">
+        <v>67</v>
+      </c>
+      <c r="I75" t="s">
+        <v>29</v>
+      </c>
+      <c r="J75" t="s">
+        <v>116</v>
+      </c>
+      <c r="K75" t="s">
+        <v>31</v>
+      </c>
+      <c r="L75" t="s">
+        <v>25</v>
+      </c>
+      <c r="M75" t="s">
+        <v>32</v>
+      </c>
+      <c r="N75" t="n">
+        <v>5</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0.0512965190159777</v>
+      </c>
+      <c r="P75" t="n">
+        <v>0.05717478501796722</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.3949637806140048</v>
+      </c>
+      <c r="R75" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="S75" t="n">
+        <v>1.161946957174316</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1.149347641055569</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
+      <c r="A76" t="s">
+        <v>128</v>
+      </c>
+      <c r="B76" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" t="s">
+        <v>23</v>
+      </c>
+      <c r="D76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" t="s">
+        <v>26</v>
+      </c>
+      <c r="G76" t="s">
+        <v>129</v>
+      </c>
+      <c r="H76" t="s">
+        <v>67</v>
+      </c>
+      <c r="I76" t="s">
+        <v>29</v>
+      </c>
+      <c r="J76" t="s">
+        <v>116</v>
+      </c>
+      <c r="K76" t="s">
+        <v>31</v>
+      </c>
+      <c r="L76" t="s">
+        <v>25</v>
+      </c>
+      <c r="M76" t="s">
+        <v>32</v>
+      </c>
+      <c r="N76" t="n">
+        <v>4</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0.05819792332588372</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0.06103092718124389</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0.386512590548465</v>
+      </c>
+      <c r="R76" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="S76" t="n">
+        <v>1.181888736957538</v>
+      </c>
+      <c r="T76" t="n">
+        <v>1.089495295997188</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
+      <c r="A77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77" t="s">
+        <v>23</v>
+      </c>
+      <c r="D77" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" t="s">
+        <v>26</v>
+      </c>
+      <c r="G77" t="s">
+        <v>131</v>
+      </c>
+      <c r="H77" t="s">
+        <v>67</v>
+      </c>
+      <c r="I77" t="s">
+        <v>29</v>
+      </c>
+      <c r="J77" t="s">
+        <v>116</v>
+      </c>
+      <c r="K77" t="s">
+        <v>31</v>
+      </c>
+      <c r="L77" t="s">
+        <v>25</v>
+      </c>
+      <c r="M77" t="s">
+        <v>32</v>
+      </c>
+      <c r="N77" t="n">
+        <v>14</v>
+      </c>
+      <c r="O77" t="n">
+        <v>0.0412511142852924</v>
+      </c>
+      <c r="P77" t="n">
+        <v>0.08157251405715943</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0.6436702311141773</v>
+      </c>
+      <c r="R77" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="S77" t="n">
+        <v>0.7808284046993772</v>
+      </c>
+      <c r="T77" t="n">
+        <v>1.145425685062108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20">
+      <c r="A78" t="s">
+        <v>132</v>
+      </c>
+      <c r="B78" t="s">
+        <v>44</v>
+      </c>
+      <c r="C78" t="s">
+        <v>23</v>
+      </c>
+      <c r="D78" t="s">
+        <v>24</v>
+      </c>
+      <c r="E78" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G78" t="s">
+        <v>133</v>
+      </c>
+      <c r="H78" t="s">
+        <v>67</v>
+      </c>
+      <c r="I78" t="s">
+        <v>29</v>
+      </c>
+      <c r="J78" t="s">
+        <v>116</v>
+      </c>
+      <c r="K78" t="s">
+        <v>31</v>
+      </c>
+      <c r="L78" t="s">
+        <v>25</v>
+      </c>
+      <c r="M78" t="s">
+        <v>32</v>
+      </c>
+      <c r="N78" t="n">
+        <v>10</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0.06305061516658156</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0.08462496173381806</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0.482235253535702</v>
+      </c>
+      <c r="R78" t="n">
+        <v>0.361</v>
+      </c>
+      <c r="S78" t="n">
+        <v>1.019303172888945</v>
+      </c>
+      <c r="T78" t="n">
+        <v>1.068644000591404</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20">
+      <c r="A79" t="s">
+        <v>134</v>
+      </c>
+      <c r="B79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>24</v>
+      </c>
+      <c r="E79" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" t="s">
+        <v>26</v>
+      </c>
+      <c r="G79" t="s">
+        <v>135</v>
+      </c>
+      <c r="H79" t="s">
+        <v>67</v>
+      </c>
+      <c r="I79" t="s">
+        <v>29</v>
+      </c>
+      <c r="J79" t="s">
+        <v>116</v>
+      </c>
+      <c r="K79" t="s">
+        <v>31</v>
+      </c>
+      <c r="L79" t="s">
+        <v>25</v>
+      </c>
+      <c r="M79" t="s">
+        <v>32</v>
+      </c>
+      <c r="N79" t="n">
+        <v>7</v>
+      </c>
+      <c r="O79" t="n">
+        <v>0.1182613470670313</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0.1243769266605377</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0.3830631252155916</v>
+      </c>
+      <c r="R79" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="S79" t="n">
+        <v>1.125912301127835</v>
+      </c>
+      <c r="T79" t="n">
+        <v>1.050714042925096</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20">
+      <c r="A80" t="s">
+        <v>136</v>
+      </c>
+      <c r="B80" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" t="s">
+        <v>23</v>
+      </c>
+      <c r="D80" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" t="s">
+        <v>26</v>
+      </c>
+      <c r="G80" t="s">
+        <v>137</v>
+      </c>
+      <c r="H80" t="s">
+        <v>67</v>
+      </c>
+      <c r="I80" t="s">
+        <v>29</v>
+      </c>
+      <c r="J80" t="s">
+        <v>116</v>
+      </c>
+      <c r="K80" t="s">
+        <v>31</v>
+      </c>
+      <c r="L80" t="s">
+        <v>25</v>
+      </c>
+      <c r="M80" t="s">
+        <v>32</v>
+      </c>
+      <c r="N80" t="n">
+        <v>17</v>
+      </c>
+      <c r="O80" t="n">
+        <v>0.1623369806509423</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0.201347945690155</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>0.4617109348051052</v>
+      </c>
+      <c r="R80" t="n">
+        <v>0.393</v>
+      </c>
+      <c r="S80" t="n">
+        <v>0.941273164787212</v>
+      </c>
+      <c r="T80" t="n">
+        <v>1.058772874605314</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20">
+      <c r="A81" t="s">
+        <v>138</v>
+      </c>
+      <c r="B81" t="s">
+        <v>44</v>
+      </c>
+      <c r="C81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" t="s">
+        <v>25</v>
+      </c>
+      <c r="F81" t="s">
+        <v>26</v>
+      </c>
+      <c r="G81" t="s">
+        <v>125</v>
+      </c>
+      <c r="H81" t="s">
+        <v>28</v>
+      </c>
+      <c r="I81" t="s">
+        <v>29</v>
+      </c>
+      <c r="J81" t="s">
+        <v>116</v>
+      </c>
+      <c r="K81" t="s">
+        <v>31</v>
+      </c>
+      <c r="L81" t="s">
+        <v>25</v>
+      </c>
+      <c r="M81" t="s">
+        <v>32</v>
+      </c>
+      <c r="N81" t="n">
+        <v>11</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0.03990969696140322</v>
+      </c>
+      <c r="P81" t="n">
+        <v>0.04789634823799133</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>0.499482580200069</v>
+      </c>
+      <c r="R81" t="n">
+        <v>0.418</v>
+      </c>
+      <c r="S81" t="n">
+        <v>0.9987056127810362</v>
+      </c>
+      <c r="T81" t="n">
+        <v>1.079814798935447</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20">
+      <c r="A82" t="s">
+        <v>139</v>
+      </c>
+      <c r="B82" t="s">
+        <v>44</v>
+      </c>
+      <c r="C82" t="s">
+        <v>23</v>
+      </c>
+      <c r="D82" t="s">
+        <v>24</v>
+      </c>
+      <c r="E82" t="s">
+        <v>25</v>
+      </c>
+      <c r="F82" t="s">
+        <v>26</v>
+      </c>
+      <c r="G82" t="s">
+        <v>127</v>
+      </c>
+      <c r="H82" t="s">
+        <v>28</v>
+      </c>
+      <c r="I82" t="s">
+        <v>29</v>
+      </c>
+      <c r="J82" t="s">
+        <v>116</v>
+      </c>
+      <c r="K82" t="s">
+        <v>31</v>
+      </c>
+      <c r="L82" t="s">
+        <v>25</v>
+      </c>
+      <c r="M82" t="s">
+        <v>32</v>
+      </c>
+      <c r="N82" t="n">
+        <v>7</v>
+      </c>
+      <c r="O82" t="n">
+        <v>0.0522962340448346</v>
+      </c>
+      <c r="P82" t="n">
+        <v>0.05076391339302063</v>
+      </c>
+      <c r="Q82" t="n">
+        <v>0.3673680579510176</v>
+      </c>
+      <c r="R82" t="n">
+        <v>0.427</v>
+      </c>
+      <c r="S82" t="n">
+        <v>1.196032304556445</v>
+      </c>
+      <c r="T82" t="n">
+        <v>1.075639344761989</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>44</v>
+      </c>
+      <c r="C83" t="s">
+        <v>23</v>
+      </c>
+      <c r="D83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E83" t="s">
+        <v>25</v>
+      </c>
+      <c r="F83" t="s">
+        <v>26</v>
+      </c>
+      <c r="G83" t="s">
+        <v>129</v>
+      </c>
+      <c r="H83" t="s">
+        <v>28</v>
+      </c>
+      <c r="I83" t="s">
+        <v>29</v>
+      </c>
+      <c r="J83" t="s">
+        <v>116</v>
+      </c>
+      <c r="K83" t="s">
+        <v>31</v>
+      </c>
+      <c r="L83" t="s">
+        <v>25</v>
+      </c>
+      <c r="M83" t="s">
+        <v>32</v>
+      </c>
+      <c r="N83" t="n">
+        <v>13</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0.05331991700807001</v>
+      </c>
+      <c r="P83" t="n">
+        <v>0.05716223275661469</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>0.4379096240082787</v>
+      </c>
+      <c r="R83" t="n">
+        <v>0.407</v>
+      </c>
+      <c r="S83" t="n">
+        <v>1.054237985585708</v>
+      </c>
+      <c r="T83" t="n">
+        <v>1.088577052853862</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20">
+      <c r="A84" t="s">
+        <v>141</v>
+      </c>
+      <c r="B84" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D84" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" t="s">
+        <v>25</v>
+      </c>
+      <c r="F84" t="s">
+        <v>26</v>
+      </c>
+      <c r="G84" t="s">
+        <v>131</v>
+      </c>
+      <c r="H84" t="s">
+        <v>28</v>
+      </c>
+      <c r="I84" t="s">
+        <v>29</v>
+      </c>
+      <c r="J84" t="s">
+        <v>116</v>
+      </c>
+      <c r="K84" t="s">
+        <v>31</v>
+      </c>
+      <c r="L84" t="s">
+        <v>25</v>
+      </c>
+      <c r="M84" t="s">
+        <v>32</v>
+      </c>
+      <c r="N84" t="n">
+        <v>4</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0.07165291357468062</v>
+      </c>
+      <c r="P84" t="n">
+        <v>0.07204147017002106</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0.3258020006898931</v>
+      </c>
+      <c r="R84" t="n">
+        <v>0.346</v>
+      </c>
+      <c r="S84" t="n">
+        <v>1.286890945772998</v>
+      </c>
+      <c r="T84" t="n">
+        <v>1.07144761887831</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20">
+      <c r="A85" t="s">
+        <v>142</v>
+      </c>
+      <c r="B85" t="s">
+        <v>44</v>
+      </c>
+      <c r="C85" t="s">
+        <v>23</v>
+      </c>
+      <c r="D85" t="s">
+        <v>24</v>
+      </c>
+      <c r="E85" t="s">
+        <v>25</v>
+      </c>
+      <c r="F85" t="s">
+        <v>26</v>
+      </c>
+      <c r="G85" t="s">
+        <v>133</v>
+      </c>
+      <c r="H85" t="s">
+        <v>28</v>
+      </c>
+      <c r="I85" t="s">
+        <v>29</v>
+      </c>
+      <c r="J85" t="s">
+        <v>116</v>
+      </c>
+      <c r="K85" t="s">
+        <v>31</v>
+      </c>
+      <c r="L85" t="s">
+        <v>25</v>
+      </c>
+      <c r="M85" t="s">
+        <v>32</v>
+      </c>
+      <c r="N85" t="n">
+        <v>12</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0.06449630806140959</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0.07256469130516052</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0.4596412556053812</v>
+      </c>
+      <c r="R85" t="n">
+        <v>0.386</v>
+      </c>
+      <c r="S85" t="n">
+        <v>0.9812839791169582</v>
+      </c>
+      <c r="T85" t="n">
+        <v>1.056409011699541</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20">
+      <c r="A86" t="s">
+        <v>143</v>
+      </c>
+      <c r="B86" t="s">
+        <v>44</v>
+      </c>
+      <c r="C86" t="s">
+        <v>23</v>
+      </c>
+      <c r="D86" t="s">
+        <v>24</v>
+      </c>
+      <c r="E86" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" t="s">
+        <v>26</v>
+      </c>
+      <c r="G86" t="s">
+        <v>135</v>
+      </c>
+      <c r="H86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" t="s">
+        <v>29</v>
+      </c>
+      <c r="J86" t="s">
+        <v>116</v>
+      </c>
+      <c r="K86" t="s">
+        <v>31</v>
+      </c>
+      <c r="L86" t="s">
+        <v>25</v>
+      </c>
+      <c r="M86" t="s">
+        <v>32</v>
+      </c>
+      <c r="N86" t="n">
+        <v>12</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0.1189251463344978</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0.1241101398468018</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>0.3770265608830631</v>
+      </c>
+      <c r="R86" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="S86" t="n">
+        <v>1.101677982611756</v>
+      </c>
+      <c r="T86" t="n">
+        <v>1.087658034494298</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20">
+      <c r="A87" t="s">
+        <v>144</v>
+      </c>
+      <c r="B87" t="s">
+        <v>44</v>
+      </c>
+      <c r="C87" t="s">
+        <v>23</v>
+      </c>
+      <c r="D87" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" t="s">
+        <v>25</v>
+      </c>
+      <c r="F87" t="s">
+        <v>26</v>
+      </c>
+      <c r="G87" t="s">
+        <v>137</v>
+      </c>
+      <c r="H87" t="s">
+        <v>28</v>
+      </c>
+      <c r="I87" t="s">
+        <v>29</v>
+      </c>
+      <c r="J87" t="s">
+        <v>116</v>
+      </c>
+      <c r="K87" t="s">
+        <v>31</v>
+      </c>
+      <c r="L87" t="s">
+        <v>25</v>
+      </c>
+      <c r="M87" t="s">
+        <v>32</v>
+      </c>
+      <c r="N87" t="n">
+        <v>12</v>
+      </c>
+      <c r="O87" t="n">
+        <v>0.2012024506407386</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0.2039953980445862</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>0.3521904104863746</v>
+      </c>
+      <c r="R87" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="S87" t="n">
+        <v>1.121230413682091</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1.083512805646523</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20">
+      <c r="A88" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" t="s">
+        <v>44</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" t="s">
+        <v>25</v>
+      </c>
+      <c r="F88" t="s">
+        <v>26</v>
+      </c>
+      <c r="G88" t="s">
+        <v>125</v>
+      </c>
+      <c r="H88" t="s">
+        <v>60</v>
+      </c>
+      <c r="I88" t="s">
+        <v>29</v>
+      </c>
+      <c r="J88" t="s">
+        <v>116</v>
+      </c>
+      <c r="K88" t="s">
+        <v>31</v>
+      </c>
+      <c r="L88" t="s">
+        <v>25</v>
+      </c>
+      <c r="M88" t="s">
+        <v>32</v>
+      </c>
+      <c r="N88" t="n">
+        <v>21</v>
+      </c>
+      <c r="O88" t="n">
+        <v>0.05010886420953599</v>
+      </c>
+      <c r="P88" t="n">
+        <v>0.0505552841424942</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>0.3359779234218696</v>
+      </c>
+      <c r="R88" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="S88" t="n">
+        <v>1.207299290319371</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1.172177460967408</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20">
+      <c r="A89" t="s">
+        <v>146</v>
+      </c>
+      <c r="B89" t="s">
+        <v>44</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" t="s">
+        <v>26</v>
+      </c>
+      <c r="G89" t="s">
+        <v>127</v>
+      </c>
+      <c r="H89" t="s">
+        <v>60</v>
+      </c>
+      <c r="I89" t="s">
+        <v>29</v>
+      </c>
+      <c r="J89" t="s">
+        <v>116</v>
+      </c>
+      <c r="K89" t="s">
+        <v>31</v>
+      </c>
+      <c r="L89" t="s">
+        <v>25</v>
+      </c>
+      <c r="M89" t="s">
+        <v>32</v>
+      </c>
+      <c r="N89" t="n">
+        <v>12</v>
+      </c>
+      <c r="O89" t="n">
+        <v>0.05650973063002129</v>
+      </c>
+      <c r="P89" t="n">
+        <v>0.05652736580371857</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>0.3147637116246982</v>
+      </c>
+      <c r="R89" t="n">
+        <v>0.335</v>
+      </c>
+      <c r="S89" t="n">
+        <v>1.255618624579052</v>
+      </c>
+      <c r="T89" t="n">
+        <v>1.211197754291181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20">
+      <c r="A90" t="s">
+        <v>147</v>
+      </c>
+      <c r="B90" t="s">
+        <v>44</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" t="s">
+        <v>24</v>
+      </c>
+      <c r="E90" t="s">
+        <v>25</v>
+      </c>
+      <c r="F90" t="s">
+        <v>26</v>
+      </c>
+      <c r="G90" t="s">
+        <v>129</v>
+      </c>
+      <c r="H90" t="s">
+        <v>60</v>
+      </c>
+      <c r="I90" t="s">
+        <v>29</v>
+      </c>
+      <c r="J90" t="s">
+        <v>116</v>
+      </c>
+      <c r="K90" t="s">
+        <v>31</v>
+      </c>
+      <c r="L90" t="s">
+        <v>25</v>
+      </c>
+      <c r="M90" t="s">
+        <v>32</v>
+      </c>
+      <c r="N90" t="n">
+        <v>19</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0.06315722254565273</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0.06361057186126709</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>0.3113142462918247</v>
+      </c>
+      <c r="R90" t="n">
+        <v>0.323</v>
+      </c>
+      <c r="S90" t="n">
+        <v>1.231135681906984</v>
+      </c>
+      <c r="T90" t="n">
+        <v>1.180254209905646</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20">
+      <c r="A91" t="s">
+        <v>148</v>
+      </c>
+      <c r="B91" t="s">
+        <v>44</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91" t="s">
+        <v>24</v>
+      </c>
+      <c r="E91" t="s">
+        <v>25</v>
+      </c>
+      <c r="F91" t="s">
+        <v>26</v>
+      </c>
+      <c r="G91" t="s">
+        <v>131</v>
+      </c>
+      <c r="H91" t="s">
+        <v>60</v>
+      </c>
+      <c r="I91" t="s">
+        <v>29</v>
+      </c>
+      <c r="J91" t="s">
+        <v>116</v>
+      </c>
+      <c r="K91" t="s">
+        <v>31</v>
+      </c>
+      <c r="L91" t="s">
+        <v>25</v>
+      </c>
+      <c r="M91" t="s">
+        <v>32</v>
+      </c>
+      <c r="N91" t="n">
+        <v>23</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0.07028833684447552</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0.07072005212306977</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0.3308037254225595</v>
+      </c>
+      <c r="R91" t="n">
+        <v>0.328</v>
+      </c>
+      <c r="S91" t="n">
+        <v>1.194011734480268</v>
+      </c>
+      <c r="T91" t="n">
+        <v>1.166619046647191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20">
+      <c r="A92" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" t="s">
+        <v>44</v>
+      </c>
+      <c r="C92" t="s">
+        <v>23</v>
+      </c>
+      <c r="D92" t="s">
+        <v>24</v>
+      </c>
+      <c r="E92" t="s">
+        <v>25</v>
+      </c>
+      <c r="F92" t="s">
+        <v>26</v>
+      </c>
+      <c r="G92" t="s">
+        <v>133</v>
+      </c>
+      <c r="H92" t="s">
+        <v>60</v>
+      </c>
+      <c r="I92" t="s">
+        <v>29</v>
+      </c>
+      <c r="J92" t="s">
+        <v>116</v>
+      </c>
+      <c r="K92" t="s">
+        <v>31</v>
+      </c>
+      <c r="L92" t="s">
+        <v>25</v>
+      </c>
+      <c r="M92" t="s">
+        <v>32</v>
+      </c>
+      <c r="N92" t="n">
+        <v>16</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0.07888493491847501</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0.07932741284370422</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>0.3333908244222146</v>
+      </c>
+      <c r="R92" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="S92" t="n">
+        <v>1.202288837068947</v>
+      </c>
+      <c r="T92" t="n">
+        <v>1.136661779070626</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20">
+      <c r="A93" t="s">
+        <v>150</v>
+      </c>
+      <c r="B93" t="s">
+        <v>44</v>
+      </c>
+      <c r="C93" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" t="s">
+        <v>24</v>
+      </c>
+      <c r="E93" t="s">
+        <v>25</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
+      </c>
+      <c r="G93" t="s">
+        <v>135</v>
+      </c>
+      <c r="H93" t="s">
+        <v>60</v>
+      </c>
+      <c r="I93" t="s">
+        <v>29</v>
+      </c>
+      <c r="J93" t="s">
+        <v>116</v>
+      </c>
+      <c r="K93" t="s">
+        <v>31</v>
+      </c>
+      <c r="L93" t="s">
+        <v>25</v>
+      </c>
+      <c r="M93" t="s">
+        <v>32</v>
+      </c>
+      <c r="N93" t="n">
+        <v>16</v>
+      </c>
+      <c r="O93" t="n">
+        <v>0.1311076536964819</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0.1309295251369476</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>0.3109692997585374</v>
+      </c>
+      <c r="R93" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="S93" t="n">
+        <v>1.218249752501014</v>
+      </c>
+      <c r="T93" t="n">
+        <v>1.158447236605966</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20">
+      <c r="A94" t="s">
+        <v>151</v>
+      </c>
+      <c r="B94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C94" t="s">
+        <v>23</v>
+      </c>
+      <c r="D94" t="s">
+        <v>24</v>
+      </c>
+      <c r="E94" t="s">
+        <v>25</v>
+      </c>
+      <c r="F94" t="s">
+        <v>26</v>
+      </c>
+      <c r="G94" t="s">
+        <v>137</v>
+      </c>
+      <c r="H94" t="s">
+        <v>60</v>
+      </c>
+      <c r="I94" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" t="s">
+        <v>116</v>
+      </c>
+      <c r="K94" t="s">
+        <v>31</v>
+      </c>
+      <c r="L94" t="s">
+        <v>25</v>
+      </c>
+      <c r="M94" t="s">
+        <v>32</v>
+      </c>
+      <c r="N94" t="n">
+        <v>13</v>
+      </c>
+      <c r="O94" t="n">
+        <v>0.2135896431079771</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0.216498514175415</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>0.3121766126250431</v>
+      </c>
+      <c r="R94" t="n">
+        <v>0.321</v>
+      </c>
+      <c r="S94" t="n">
+        <v>1.207584974017246</v>
+      </c>
+      <c r="T94" t="n">
+        <v>1.152388823271035</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20">
+      <c r="A95" t="s">
+        <v>152</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" t="s">
+        <v>23</v>
+      </c>
+      <c r="D95" t="s">
+        <v>24</v>
+      </c>
+      <c r="E95" t="s">
+        <v>25</v>
+      </c>
+      <c r="F95" t="s">
+        <v>26</v>
+      </c>
+      <c r="G95" t="s">
+        <v>153</v>
+      </c>
+      <c r="H95" t="s">
+        <v>28</v>
+      </c>
+      <c r="I95" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" t="s">
+        <v>154</v>
+      </c>
+      <c r="K95" t="s">
+        <v>31</v>
+      </c>
+      <c r="L95" t="s">
+        <v>25</v>
+      </c>
+      <c r="M95" t="s">
+        <v>155</v>
+      </c>
+      <c r="N95" t="n">
+        <v>7</v>
+      </c>
+      <c r="O95" t="n">
+        <v>0.01658145507081385</v>
+      </c>
+      <c r="P95" t="n">
+        <v>0.01679799503087998</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>0.5228982150722919</v>
+      </c>
+      <c r="R95" t="n">
+        <v>0.524</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0.9655517642023744</v>
+      </c>
+      <c r="T95" t="n">
+        <v>0.9777525249264253</v>
+      </c>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Slight modifications, addition of the new validation set
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="204">
   <si>
     <t>Date</t>
   </si>
@@ -527,6 +527,105 @@
   </si>
   <si>
     <t>September20  12:38:30</t>
+  </si>
+  <si>
+    <t>September25  18:01:38</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fb7a2408840&gt;</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>September25  18:02:04</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fb7a24087b8&gt;</t>
+  </si>
+  <si>
+    <t>September25  18:03:52</t>
+  </si>
+  <si>
+    <t>September25  18:08:53</t>
+  </si>
+  <si>
+    <t>1.0xsingle + 0.0Xmulti</t>
+  </si>
+  <si>
+    <t>September25  18:15:52</t>
+  </si>
+  <si>
+    <t>September25  18:17:25</t>
+  </si>
+  <si>
+    <t>September25  18:18:11</t>
+  </si>
+  <si>
+    <t>September25  18:22:37</t>
+  </si>
+  <si>
+    <t>September25  18:27:20</t>
+  </si>
+  <si>
+    <t>September25  18:32:12</t>
+  </si>
+  <si>
+    <t>September25  18:33:18</t>
+  </si>
+  <si>
+    <t>September25  18:33:39</t>
+  </si>
+  <si>
+    <t>September25  18:34:54</t>
+  </si>
+  <si>
+    <t>September25  18:42:46</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f0d4bb63840&gt;</t>
+  </si>
+  <si>
+    <t>September28  18:12:40</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f4b85717ea0&gt;</t>
+  </si>
+  <si>
+    <t>September28  18:13:49</t>
+  </si>
+  <si>
+    <t>September28  18:21:34</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fb8d691f8c8&gt;</t>
+  </si>
+  <si>
+    <t>September28  18:32:14</t>
+  </si>
+  <si>
+    <t>September28  18:46:01</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fde41d558c8&gt;</t>
+  </si>
+  <si>
+    <t>September28  18:47:56</t>
+  </si>
+  <si>
+    <t>September28  18:49:10</t>
+  </si>
+  <si>
+    <t>October04  22:26:39</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fd3688c7a60&gt;</t>
+  </si>
+  <si>
+    <t>October04  22:28:17</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f303bf42a60&gt;</t>
   </si>
 </sst>
 </file>
@@ -904,7 +1003,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y100"/>
+  <dimension ref="A1:Y123"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="H1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="X13" activeCellId="0" pane="topLeft" sqref="X13"/>
@@ -6866,6 +6965,1447 @@
         <v>25</v>
       </c>
     </row>
+    <row r="101" spans="1:25">
+      <c r="A101" t="s">
+        <v>171</v>
+      </c>
+      <c r="B101" t="s">
+        <v>49</v>
+      </c>
+      <c r="C101" t="s">
+        <v>28</v>
+      </c>
+      <c r="D101" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" t="s">
+        <v>30</v>
+      </c>
+      <c r="F101" t="s">
+        <v>31</v>
+      </c>
+      <c r="G101" t="s">
+        <v>168</v>
+      </c>
+      <c r="H101" t="s">
+        <v>33</v>
+      </c>
+      <c r="I101" t="s">
+        <v>34</v>
+      </c>
+      <c r="J101" t="s">
+        <v>172</v>
+      </c>
+      <c r="K101" t="s">
+        <v>36</v>
+      </c>
+      <c r="L101" t="s">
+        <v>30</v>
+      </c>
+      <c r="M101" t="s">
+        <v>173</v>
+      </c>
+      <c r="S101" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:25">
+      <c r="A102" t="s">
+        <v>174</v>
+      </c>
+      <c r="B102" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" t="s">
+        <v>28</v>
+      </c>
+      <c r="D102" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" t="s">
+        <v>30</v>
+      </c>
+      <c r="F102" t="s">
+        <v>31</v>
+      </c>
+      <c r="G102" t="s">
+        <v>168</v>
+      </c>
+      <c r="H102" t="s">
+        <v>33</v>
+      </c>
+      <c r="I102" t="s">
+        <v>34</v>
+      </c>
+      <c r="J102" t="s">
+        <v>175</v>
+      </c>
+      <c r="K102" t="s">
+        <v>36</v>
+      </c>
+      <c r="L102" t="s">
+        <v>30</v>
+      </c>
+      <c r="M102" t="s">
+        <v>173</v>
+      </c>
+      <c r="S102" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:25">
+      <c r="A103" t="s">
+        <v>176</v>
+      </c>
+      <c r="B103" t="s">
+        <v>49</v>
+      </c>
+      <c r="C103" t="s">
+        <v>28</v>
+      </c>
+      <c r="D103" t="s">
+        <v>29</v>
+      </c>
+      <c r="E103" t="s">
+        <v>30</v>
+      </c>
+      <c r="F103" t="s">
+        <v>31</v>
+      </c>
+      <c r="G103" t="s">
+        <v>168</v>
+      </c>
+      <c r="H103" t="s">
+        <v>33</v>
+      </c>
+      <c r="I103" t="s">
+        <v>34</v>
+      </c>
+      <c r="J103" t="s">
+        <v>175</v>
+      </c>
+      <c r="K103" t="s">
+        <v>36</v>
+      </c>
+      <c r="L103" t="s">
+        <v>30</v>
+      </c>
+      <c r="M103" t="s">
+        <v>173</v>
+      </c>
+      <c r="N103" t="n">
+        <v>13</v>
+      </c>
+      <c r="O103" t="n">
+        <v>0.0079049546426783</v>
+      </c>
+      <c r="P103" t="n">
+        <v>0.02518401054897569</v>
+      </c>
+      <c r="Q103" t="n">
+        <v>0.5755208333333334</v>
+      </c>
+      <c r="R103" t="n">
+        <v>0.3829787234042553</v>
+      </c>
+      <c r="S103" t="n">
+        <v>0.733321496116585</v>
+      </c>
+      <c r="T103" t="n">
+        <v>1.26443038342523</v>
+      </c>
+      <c r="U103" t="n">
+        <v>13</v>
+      </c>
+      <c r="V103" t="n">
+        <v>0.5755208333333334</v>
+      </c>
+      <c r="W103" t="n">
+        <v>0.3829787234042553</v>
+      </c>
+      <c r="X103" t="n">
+        <v>0.733321496116585</v>
+      </c>
+      <c r="Y103" t="n">
+        <v>1.26443038342523</v>
+      </c>
+    </row>
+    <row r="104" spans="1:25">
+      <c r="A104" t="s">
+        <v>177</v>
+      </c>
+      <c r="B104" t="s">
+        <v>49</v>
+      </c>
+      <c r="C104" t="s">
+        <v>28</v>
+      </c>
+      <c r="D104" t="s">
+        <v>29</v>
+      </c>
+      <c r="E104" t="s">
+        <v>30</v>
+      </c>
+      <c r="F104" t="s">
+        <v>31</v>
+      </c>
+      <c r="G104" t="s">
+        <v>178</v>
+      </c>
+      <c r="H104" t="s">
+        <v>33</v>
+      </c>
+      <c r="I104" t="s">
+        <v>34</v>
+      </c>
+      <c r="J104" t="s">
+        <v>175</v>
+      </c>
+      <c r="K104" t="s">
+        <v>36</v>
+      </c>
+      <c r="L104" t="s">
+        <v>30</v>
+      </c>
+      <c r="M104" t="s">
+        <v>173</v>
+      </c>
+      <c r="N104" t="n">
+        <v>20</v>
+      </c>
+      <c r="O104" t="n">
+        <v>0.04323956785568347</v>
+      </c>
+      <c r="P104" t="n">
+        <v>0.1327234439574476</v>
+      </c>
+      <c r="Q104" t="n">
+        <v>0.7421875</v>
+      </c>
+      <c r="R104" t="n">
+        <v>0.425531914893617</v>
+      </c>
+      <c r="S104" t="n">
+        <v>0.9319278852643768</v>
+      </c>
+      <c r="T104" t="n">
+        <v>1.439773707312186</v>
+      </c>
+      <c r="U104" t="n">
+        <v>20</v>
+      </c>
+      <c r="V104" t="n">
+        <v>0.7421875</v>
+      </c>
+      <c r="W104" t="n">
+        <v>0.425531914893617</v>
+      </c>
+      <c r="X104" t="n">
+        <v>0.9319278852643768</v>
+      </c>
+      <c r="Y104" t="n">
+        <v>1.439773707312186</v>
+      </c>
+    </row>
+    <row r="105" spans="1:25">
+      <c r="A105" t="s">
+        <v>179</v>
+      </c>
+      <c r="B105" t="s">
+        <v>49</v>
+      </c>
+      <c r="C105" t="s">
+        <v>28</v>
+      </c>
+      <c r="D105" t="s">
+        <v>29</v>
+      </c>
+      <c r="E105" t="s">
+        <v>30</v>
+      </c>
+      <c r="F105" t="s">
+        <v>31</v>
+      </c>
+      <c r="G105" t="s">
+        <v>178</v>
+      </c>
+      <c r="H105" t="s">
+        <v>33</v>
+      </c>
+      <c r="I105" t="s">
+        <v>34</v>
+      </c>
+      <c r="J105" t="s">
+        <v>175</v>
+      </c>
+      <c r="K105" t="s">
+        <v>36</v>
+      </c>
+      <c r="L105" t="s">
+        <v>30</v>
+      </c>
+      <c r="M105" t="s">
+        <v>173</v>
+      </c>
+      <c r="N105" t="n">
+        <v>4</v>
+      </c>
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="n">
+        <v>0.13671875</v>
+      </c>
+      <c r="R105" t="n">
+        <v>0.121580547112462</v>
+      </c>
+      <c r="S105" t="n">
+        <v>3.552801124934146</v>
+      </c>
+      <c r="T105" t="n">
+        <v>3.536608373031219</v>
+      </c>
+      <c r="U105" t="n">
+        <v>4</v>
+      </c>
+      <c r="V105" t="n">
+        <v>0.13671875</v>
+      </c>
+      <c r="W105" t="n">
+        <v>0.121580547112462</v>
+      </c>
+      <c r="X105" t="n">
+        <v>3.552801124934146</v>
+      </c>
+      <c r="Y105" t="n">
+        <v>3.536608373031219</v>
+      </c>
+    </row>
+    <row r="106" spans="1:25">
+      <c r="A106" t="s">
+        <v>180</v>
+      </c>
+      <c r="B106" t="s">
+        <v>49</v>
+      </c>
+      <c r="C106" t="s">
+        <v>28</v>
+      </c>
+      <c r="D106" t="s">
+        <v>29</v>
+      </c>
+      <c r="E106" t="s">
+        <v>30</v>
+      </c>
+      <c r="F106" t="s">
+        <v>31</v>
+      </c>
+      <c r="G106" t="s">
+        <v>178</v>
+      </c>
+      <c r="H106" t="s">
+        <v>33</v>
+      </c>
+      <c r="I106" t="s">
+        <v>34</v>
+      </c>
+      <c r="J106" t="s">
+        <v>175</v>
+      </c>
+      <c r="K106" t="s">
+        <v>36</v>
+      </c>
+      <c r="L106" t="s">
+        <v>30</v>
+      </c>
+      <c r="M106" t="s">
+        <v>173</v>
+      </c>
+      <c r="N106" t="n">
+        <v>2</v>
+      </c>
+      <c r="O106" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="n">
+        <v>0.1041666666666667</v>
+      </c>
+      <c r="R106" t="n">
+        <v>0.1155015197568389</v>
+      </c>
+      <c r="S106" t="n">
+        <v>3.219609513072458</v>
+      </c>
+      <c r="T106" t="n">
+        <v>3.356253519919138</v>
+      </c>
+      <c r="U106" t="n">
+        <v>2</v>
+      </c>
+      <c r="V106" t="n">
+        <v>0.1041666666666667</v>
+      </c>
+      <c r="W106" t="n">
+        <v>0.1155015197568389</v>
+      </c>
+      <c r="X106" t="n">
+        <v>3.219609513072458</v>
+      </c>
+      <c r="Y106" t="n">
+        <v>3.356253519919138</v>
+      </c>
+    </row>
+    <row r="107" spans="1:25">
+      <c r="A107" t="s">
+        <v>181</v>
+      </c>
+      <c r="B107" t="s">
+        <v>49</v>
+      </c>
+      <c r="C107" t="s">
+        <v>28</v>
+      </c>
+      <c r="D107" t="s">
+        <v>29</v>
+      </c>
+      <c r="E107" t="s">
+        <v>30</v>
+      </c>
+      <c r="F107" t="s">
+        <v>31</v>
+      </c>
+      <c r="G107" t="s">
+        <v>178</v>
+      </c>
+      <c r="H107" t="s">
+        <v>33</v>
+      </c>
+      <c r="I107" t="s">
+        <v>34</v>
+      </c>
+      <c r="J107" t="s">
+        <v>175</v>
+      </c>
+      <c r="K107" t="s">
+        <v>36</v>
+      </c>
+      <c r="L107" t="s">
+        <v>30</v>
+      </c>
+      <c r="M107" t="s">
+        <v>173</v>
+      </c>
+      <c r="N107" t="n">
+        <v>12</v>
+      </c>
+      <c r="O107" t="n">
+        <v>0.002769226039769516</v>
+      </c>
+      <c r="P107" t="n">
+        <v>0.01200845931574566</v>
+      </c>
+      <c r="Q107" t="n">
+        <v>0.89453125</v>
+      </c>
+      <c r="R107" t="n">
+        <v>0.4620060790273556</v>
+      </c>
+      <c r="S107" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="T107" t="n">
+        <v>1.241383677454499</v>
+      </c>
+      <c r="U107" t="n">
+        <v>12</v>
+      </c>
+      <c r="V107" t="n">
+        <v>0.89453125</v>
+      </c>
+      <c r="W107" t="n">
+        <v>0.4620060790273556</v>
+      </c>
+      <c r="X107" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="Y107" t="n">
+        <v>1.241383677454499</v>
+      </c>
+    </row>
+    <row r="108" spans="1:25">
+      <c r="A108" t="s">
+        <v>182</v>
+      </c>
+      <c r="B108" t="s">
+        <v>49</v>
+      </c>
+      <c r="C108" t="s">
+        <v>28</v>
+      </c>
+      <c r="D108" t="s">
+        <v>29</v>
+      </c>
+      <c r="E108" t="s">
+        <v>30</v>
+      </c>
+      <c r="F108" t="s">
+        <v>31</v>
+      </c>
+      <c r="G108" t="s">
+        <v>178</v>
+      </c>
+      <c r="H108" t="s">
+        <v>33</v>
+      </c>
+      <c r="I108" t="s">
+        <v>34</v>
+      </c>
+      <c r="J108" t="s">
+        <v>175</v>
+      </c>
+      <c r="K108" t="s">
+        <v>36</v>
+      </c>
+      <c r="L108" t="s">
+        <v>30</v>
+      </c>
+      <c r="M108" t="s">
+        <v>173</v>
+      </c>
+      <c r="N108" t="n">
+        <v>10</v>
+      </c>
+      <c r="O108" t="n">
+        <v>0.002782941594584069</v>
+      </c>
+      <c r="P108" t="n">
+        <v>0.004269491130978684</v>
+      </c>
+      <c r="Q108" t="n">
+        <v>0.4479166666666667</v>
+      </c>
+      <c r="R108" t="n">
+        <v>0.3860182370820669</v>
+      </c>
+      <c r="S108" t="n">
+        <v>1.001951221367587</v>
+      </c>
+      <c r="T108" t="n">
+        <v>1.214151610688962</v>
+      </c>
+      <c r="U108" t="n">
+        <v>10</v>
+      </c>
+      <c r="V108" t="n">
+        <v>0.4479166666666667</v>
+      </c>
+      <c r="W108" t="n">
+        <v>0.3860182370820669</v>
+      </c>
+      <c r="X108" t="n">
+        <v>1.001951221367587</v>
+      </c>
+      <c r="Y108" t="n">
+        <v>1.214151610688962</v>
+      </c>
+    </row>
+    <row r="109" spans="1:25">
+      <c r="A109" t="s">
+        <v>183</v>
+      </c>
+      <c r="B109" t="s">
+        <v>49</v>
+      </c>
+      <c r="C109" t="s">
+        <v>28</v>
+      </c>
+      <c r="D109" t="s">
+        <v>29</v>
+      </c>
+      <c r="E109" t="s">
+        <v>30</v>
+      </c>
+      <c r="F109" t="s">
+        <v>31</v>
+      </c>
+      <c r="G109" t="s">
+        <v>178</v>
+      </c>
+      <c r="H109" t="s">
+        <v>33</v>
+      </c>
+      <c r="I109" t="s">
+        <v>34</v>
+      </c>
+      <c r="J109" t="s">
+        <v>175</v>
+      </c>
+      <c r="K109" t="s">
+        <v>36</v>
+      </c>
+      <c r="L109" t="s">
+        <v>30</v>
+      </c>
+      <c r="M109" t="s">
+        <v>173</v>
+      </c>
+      <c r="N109" t="n">
+        <v>18</v>
+      </c>
+      <c r="O109" t="n">
+        <v>0.002259189934799603</v>
+      </c>
+      <c r="P109" t="n">
+        <v>0.004330871043596586</v>
+      </c>
+      <c r="Q109" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="R109" t="n">
+        <v>0.4316109422492401</v>
+      </c>
+      <c r="S109" t="n">
+        <v>0.7525996611745185</v>
+      </c>
+      <c r="T109" t="n">
+        <v>1.215402668837128</v>
+      </c>
+      <c r="U109" t="n">
+        <v>18</v>
+      </c>
+      <c r="V109" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="W109" t="n">
+        <v>0.4316109422492401</v>
+      </c>
+      <c r="X109" t="n">
+        <v>0.7525996611745185</v>
+      </c>
+      <c r="Y109" t="n">
+        <v>1.215402668837128</v>
+      </c>
+    </row>
+    <row r="110" spans="1:25">
+      <c r="A110" t="s">
+        <v>184</v>
+      </c>
+      <c r="B110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" t="s">
+        <v>28</v>
+      </c>
+      <c r="D110" t="s">
+        <v>29</v>
+      </c>
+      <c r="E110" t="s">
+        <v>30</v>
+      </c>
+      <c r="F110" t="s">
+        <v>31</v>
+      </c>
+      <c r="G110" t="s">
+        <v>168</v>
+      </c>
+      <c r="H110" t="s">
+        <v>33</v>
+      </c>
+      <c r="I110" t="s">
+        <v>34</v>
+      </c>
+      <c r="J110" t="s">
+        <v>175</v>
+      </c>
+      <c r="K110" t="s">
+        <v>36</v>
+      </c>
+      <c r="L110" t="s">
+        <v>30</v>
+      </c>
+      <c r="M110" t="s">
+        <v>173</v>
+      </c>
+      <c r="N110" t="n">
+        <v>5</v>
+      </c>
+      <c r="O110" t="n">
+        <v>0.01706836840215449</v>
+      </c>
+      <c r="P110" t="n">
+        <v>0.02383613747213387</v>
+      </c>
+      <c r="Q110" t="n">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="R110" t="n">
+        <v>0.3586626139817629</v>
+      </c>
+      <c r="S110" t="n">
+        <v>1.012937148428602</v>
+      </c>
+      <c r="T110" t="n">
+        <v>1.372770366901603</v>
+      </c>
+      <c r="U110" t="n">
+        <v>5</v>
+      </c>
+      <c r="V110" t="n">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="W110" t="n">
+        <v>0.3586626139817629</v>
+      </c>
+      <c r="X110" t="n">
+        <v>1.012937148428602</v>
+      </c>
+      <c r="Y110" t="n">
+        <v>1.372770366901603</v>
+      </c>
+    </row>
+    <row r="111" spans="1:25">
+      <c r="A111" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" t="s">
+        <v>49</v>
+      </c>
+      <c r="C111" t="s">
+        <v>28</v>
+      </c>
+      <c r="D111" t="s">
+        <v>29</v>
+      </c>
+      <c r="E111" t="s">
+        <v>30</v>
+      </c>
+      <c r="F111" t="s">
+        <v>31</v>
+      </c>
+      <c r="G111" t="s">
+        <v>178</v>
+      </c>
+      <c r="H111" t="s">
+        <v>33</v>
+      </c>
+      <c r="I111" t="s">
+        <v>34</v>
+      </c>
+      <c r="J111" t="s">
+        <v>175</v>
+      </c>
+      <c r="K111" t="s">
+        <v>36</v>
+      </c>
+      <c r="L111" t="s">
+        <v>30</v>
+      </c>
+      <c r="M111" t="s">
+        <v>173</v>
+      </c>
+      <c r="N111" t="n">
+        <v>1</v>
+      </c>
+      <c r="O111" t="n">
+        <v>0.007602096787498643</v>
+      </c>
+      <c r="P111" t="n">
+        <v>0.006338213635523631</v>
+      </c>
+      <c r="Q111" t="n">
+        <v>0.2057291666666667</v>
+      </c>
+      <c r="R111" t="n">
+        <v>0.2644376899696049</v>
+      </c>
+      <c r="S111" t="n">
+        <v>2.590547722007838</v>
+      </c>
+      <c r="T111" t="n">
+        <v>2.049538460906641</v>
+      </c>
+      <c r="U111" t="n">
+        <v>1</v>
+      </c>
+      <c r="V111" t="n">
+        <v>0.2057291666666667</v>
+      </c>
+      <c r="W111" t="n">
+        <v>0.2644376899696049</v>
+      </c>
+      <c r="X111" t="n">
+        <v>2.590547722007838</v>
+      </c>
+      <c r="Y111" t="n">
+        <v>2.049538460906641</v>
+      </c>
+    </row>
+    <row r="112" spans="1:25">
+      <c r="A112" t="s">
+        <v>186</v>
+      </c>
+      <c r="B112" t="s">
+        <v>49</v>
+      </c>
+      <c r="C112" t="s">
+        <v>28</v>
+      </c>
+      <c r="D112" t="s">
+        <v>29</v>
+      </c>
+      <c r="E112" t="s">
+        <v>30</v>
+      </c>
+      <c r="F112" t="s">
+        <v>31</v>
+      </c>
+      <c r="G112" t="s">
+        <v>178</v>
+      </c>
+      <c r="H112" t="s">
+        <v>33</v>
+      </c>
+      <c r="I112" t="s">
+        <v>34</v>
+      </c>
+      <c r="J112" t="s">
+        <v>175</v>
+      </c>
+      <c r="K112" t="s">
+        <v>36</v>
+      </c>
+      <c r="L112" t="s">
+        <v>30</v>
+      </c>
+      <c r="M112" t="s">
+        <v>173</v>
+      </c>
+      <c r="S112" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="113" spans="1:25">
+      <c r="A113" t="s">
+        <v>187</v>
+      </c>
+      <c r="B113" t="s">
+        <v>49</v>
+      </c>
+      <c r="C113" t="s">
+        <v>28</v>
+      </c>
+      <c r="D113" t="s">
+        <v>29</v>
+      </c>
+      <c r="E113" t="s">
+        <v>30</v>
+      </c>
+      <c r="F113" t="s">
+        <v>31</v>
+      </c>
+      <c r="G113" t="s">
+        <v>178</v>
+      </c>
+      <c r="H113" t="s">
+        <v>33</v>
+      </c>
+      <c r="I113" t="s">
+        <v>34</v>
+      </c>
+      <c r="J113" t="s">
+        <v>175</v>
+      </c>
+      <c r="K113" t="s">
+        <v>36</v>
+      </c>
+      <c r="L113" t="s">
+        <v>30</v>
+      </c>
+      <c r="M113" t="s">
+        <v>173</v>
+      </c>
+      <c r="N113" t="n">
+        <v>15</v>
+      </c>
+      <c r="O113" t="n">
+        <v>0.002433132079507535</v>
+      </c>
+      <c r="P113" t="n">
+        <v>0.003921142020644932</v>
+      </c>
+      <c r="Q113" t="n">
+        <v>0.5442708333333334</v>
+      </c>
+      <c r="R113" t="n">
+        <v>0.4012158054711246</v>
+      </c>
+      <c r="S113" t="n">
+        <v>0.8853553900364908</v>
+      </c>
+      <c r="T113" t="n">
+        <v>1.161698787529852</v>
+      </c>
+      <c r="U113" t="n">
+        <v>15</v>
+      </c>
+      <c r="V113" t="n">
+        <v>0.5442708333333334</v>
+      </c>
+      <c r="W113" t="n">
+        <v>0.4012158054711246</v>
+      </c>
+      <c r="X113" t="n">
+        <v>0.8853553900364908</v>
+      </c>
+      <c r="Y113" t="n">
+        <v>1.161698787529852</v>
+      </c>
+    </row>
+    <row r="114" spans="1:25">
+      <c r="A114" t="s">
+        <v>188</v>
+      </c>
+      <c r="B114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" t="s">
+        <v>28</v>
+      </c>
+      <c r="D114" t="s">
+        <v>29</v>
+      </c>
+      <c r="E114" t="s">
+        <v>30</v>
+      </c>
+      <c r="F114" t="s">
+        <v>31</v>
+      </c>
+      <c r="G114" t="s">
+        <v>178</v>
+      </c>
+      <c r="H114" t="s">
+        <v>33</v>
+      </c>
+      <c r="I114" t="s">
+        <v>34</v>
+      </c>
+      <c r="J114" t="s">
+        <v>189</v>
+      </c>
+      <c r="K114" t="s">
+        <v>36</v>
+      </c>
+      <c r="L114" t="s">
+        <v>30</v>
+      </c>
+      <c r="M114" t="s">
+        <v>160</v>
+      </c>
+      <c r="N114" t="n">
+        <v>13</v>
+      </c>
+      <c r="O114" t="n">
+        <v>0.0008734013459980413</v>
+      </c>
+      <c r="P114" t="n">
+        <v>0.0009759009182453155</v>
+      </c>
+      <c r="Q114" t="n">
+        <v>0.517490518523854</v>
+      </c>
+      <c r="R114" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="S114" t="n">
+        <v>0.834661159632885</v>
+      </c>
+      <c r="T114" t="n">
+        <v>0.8689073598491384</v>
+      </c>
+      <c r="U114" t="n">
+        <v>13</v>
+      </c>
+      <c r="V114" t="n">
+        <v>0.517490518523854</v>
+      </c>
+      <c r="W114" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="X114" t="n">
+        <v>0.834661159632885</v>
+      </c>
+      <c r="Y114" t="n">
+        <v>0.8689073598491384</v>
+      </c>
+    </row>
+    <row r="115" spans="1:25">
+      <c r="A115" t="s">
+        <v>190</v>
+      </c>
+      <c r="B115" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" t="s">
+        <v>28</v>
+      </c>
+      <c r="D115" t="s">
+        <v>29</v>
+      </c>
+      <c r="E115" t="s">
+        <v>30</v>
+      </c>
+      <c r="F115" t="s">
+        <v>31</v>
+      </c>
+      <c r="G115" t="s">
+        <v>168</v>
+      </c>
+      <c r="H115" t="s">
+        <v>33</v>
+      </c>
+      <c r="I115" t="s">
+        <v>34</v>
+      </c>
+      <c r="J115" t="s">
+        <v>191</v>
+      </c>
+      <c r="K115" t="s">
+        <v>36</v>
+      </c>
+      <c r="L115" t="s">
+        <v>30</v>
+      </c>
+      <c r="M115" t="s">
+        <v>160</v>
+      </c>
+      <c r="S115" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:25">
+      <c r="A116" t="s">
+        <v>192</v>
+      </c>
+      <c r="B116" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" t="s">
+        <v>28</v>
+      </c>
+      <c r="D116" t="s">
+        <v>29</v>
+      </c>
+      <c r="E116" t="s">
+        <v>30</v>
+      </c>
+      <c r="F116" t="s">
+        <v>31</v>
+      </c>
+      <c r="G116" t="s">
+        <v>168</v>
+      </c>
+      <c r="H116" t="s">
+        <v>33</v>
+      </c>
+      <c r="I116" t="s">
+        <v>34</v>
+      </c>
+      <c r="J116" t="s">
+        <v>191</v>
+      </c>
+      <c r="K116" t="s">
+        <v>36</v>
+      </c>
+      <c r="L116" t="s">
+        <v>30</v>
+      </c>
+      <c r="M116" t="s">
+        <v>173</v>
+      </c>
+      <c r="N116" t="n">
+        <v>5</v>
+      </c>
+      <c r="O116" t="n">
+        <v>0.01609985243218641</v>
+      </c>
+      <c r="P116" t="n">
+        <v>0.02417135745921033</v>
+      </c>
+      <c r="Q116" t="n">
+        <v>0.4557291666666667</v>
+      </c>
+      <c r="R116" t="n">
+        <v>0.4133738601823708</v>
+      </c>
+      <c r="S116" t="n">
+        <v>1.006489360765097</v>
+      </c>
+      <c r="T116" t="n">
+        <v>1.320863676184575</v>
+      </c>
+      <c r="U116" t="n">
+        <v>5</v>
+      </c>
+      <c r="V116" t="n">
+        <v>0.4557291666666667</v>
+      </c>
+      <c r="W116" t="n">
+        <v>0.4133738601823708</v>
+      </c>
+      <c r="X116" t="n">
+        <v>1.006489360765097</v>
+      </c>
+      <c r="Y116" t="n">
+        <v>1.320863676184575</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25">
+      <c r="A117" t="s">
+        <v>193</v>
+      </c>
+      <c r="B117" t="s">
+        <v>27</v>
+      </c>
+      <c r="C117" t="s">
+        <v>28</v>
+      </c>
+      <c r="D117" t="s">
+        <v>29</v>
+      </c>
+      <c r="E117" t="s">
+        <v>30</v>
+      </c>
+      <c r="F117" t="s">
+        <v>31</v>
+      </c>
+      <c r="G117" t="s">
+        <v>178</v>
+      </c>
+      <c r="H117" t="s">
+        <v>33</v>
+      </c>
+      <c r="I117" t="s">
+        <v>34</v>
+      </c>
+      <c r="J117" t="s">
+        <v>194</v>
+      </c>
+      <c r="K117" t="s">
+        <v>36</v>
+      </c>
+      <c r="L117" t="s">
+        <v>30</v>
+      </c>
+      <c r="M117" t="s">
+        <v>160</v>
+      </c>
+      <c r="S117" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25">
+      <c r="A118" t="s">
+        <v>195</v>
+      </c>
+      <c r="B118" t="s">
+        <v>27</v>
+      </c>
+      <c r="C118" t="s">
+        <v>28</v>
+      </c>
+      <c r="D118" t="s">
+        <v>29</v>
+      </c>
+      <c r="E118" t="s">
+        <v>30</v>
+      </c>
+      <c r="F118" t="s">
+        <v>31</v>
+      </c>
+      <c r="G118" t="s">
+        <v>178</v>
+      </c>
+      <c r="H118" t="s">
+        <v>33</v>
+      </c>
+      <c r="I118" t="s">
+        <v>34</v>
+      </c>
+      <c r="J118" t="s">
+        <v>194</v>
+      </c>
+      <c r="K118" t="s">
+        <v>36</v>
+      </c>
+      <c r="L118" t="s">
+        <v>30</v>
+      </c>
+      <c r="M118" t="s">
+        <v>160</v>
+      </c>
+      <c r="S118" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119" spans="1:25">
+      <c r="A119" t="s">
+        <v>196</v>
+      </c>
+      <c r="B119" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" t="s">
+        <v>28</v>
+      </c>
+      <c r="D119" t="s">
+        <v>29</v>
+      </c>
+      <c r="E119" t="s">
+        <v>30</v>
+      </c>
+      <c r="F119" t="s">
+        <v>31</v>
+      </c>
+      <c r="G119" t="s">
+        <v>178</v>
+      </c>
+      <c r="H119" t="s">
+        <v>33</v>
+      </c>
+      <c r="I119" t="s">
+        <v>34</v>
+      </c>
+      <c r="J119" t="s">
+        <v>197</v>
+      </c>
+      <c r="K119" t="s">
+        <v>36</v>
+      </c>
+      <c r="L119" t="s">
+        <v>30</v>
+      </c>
+      <c r="M119" t="s">
+        <v>160</v>
+      </c>
+      <c r="S119" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:25">
+      <c r="A120" t="s">
+        <v>198</v>
+      </c>
+      <c r="B120" t="s">
+        <v>27</v>
+      </c>
+      <c r="C120" t="s">
+        <v>28</v>
+      </c>
+      <c r="D120" t="s">
+        <v>29</v>
+      </c>
+      <c r="E120" t="s">
+        <v>30</v>
+      </c>
+      <c r="F120" t="s">
+        <v>31</v>
+      </c>
+      <c r="G120" t="s">
+        <v>178</v>
+      </c>
+      <c r="H120" t="s">
+        <v>33</v>
+      </c>
+      <c r="I120" t="s">
+        <v>34</v>
+      </c>
+      <c r="J120" t="s">
+        <v>197</v>
+      </c>
+      <c r="K120" t="s">
+        <v>36</v>
+      </c>
+      <c r="L120" t="s">
+        <v>30</v>
+      </c>
+      <c r="M120" t="s">
+        <v>160</v>
+      </c>
+      <c r="S120" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:25">
+      <c r="A121" t="s">
+        <v>199</v>
+      </c>
+      <c r="B121" t="s">
+        <v>27</v>
+      </c>
+      <c r="C121" t="s">
+        <v>28</v>
+      </c>
+      <c r="D121" t="s">
+        <v>29</v>
+      </c>
+      <c r="E121" t="s">
+        <v>30</v>
+      </c>
+      <c r="F121" t="s">
+        <v>31</v>
+      </c>
+      <c r="G121" t="s">
+        <v>178</v>
+      </c>
+      <c r="H121" t="s">
+        <v>33</v>
+      </c>
+      <c r="I121" t="s">
+        <v>34</v>
+      </c>
+      <c r="J121" t="s">
+        <v>197</v>
+      </c>
+      <c r="K121" t="s">
+        <v>36</v>
+      </c>
+      <c r="L121" t="s">
+        <v>30</v>
+      </c>
+      <c r="M121" t="s">
+        <v>160</v>
+      </c>
+      <c r="S121" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:25">
+      <c r="A122" t="s">
+        <v>200</v>
+      </c>
+      <c r="B122" t="s">
+        <v>27</v>
+      </c>
+      <c r="C122" t="s">
+        <v>28</v>
+      </c>
+      <c r="D122" t="s">
+        <v>29</v>
+      </c>
+      <c r="E122" t="s">
+        <v>30</v>
+      </c>
+      <c r="F122" t="s">
+        <v>31</v>
+      </c>
+      <c r="G122" t="s">
+        <v>178</v>
+      </c>
+      <c r="H122" t="s">
+        <v>33</v>
+      </c>
+      <c r="I122" t="s">
+        <v>34</v>
+      </c>
+      <c r="J122" t="s">
+        <v>201</v>
+      </c>
+      <c r="K122" t="s">
+        <v>36</v>
+      </c>
+      <c r="L122" t="s">
+        <v>30</v>
+      </c>
+      <c r="M122" t="s">
+        <v>160</v>
+      </c>
+      <c r="S122" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:25">
+      <c r="A123" t="s">
+        <v>202</v>
+      </c>
+      <c r="B123" t="s">
+        <v>27</v>
+      </c>
+      <c r="C123" t="s">
+        <v>28</v>
+      </c>
+      <c r="D123" t="s">
+        <v>29</v>
+      </c>
+      <c r="E123" t="s">
+        <v>30</v>
+      </c>
+      <c r="F123" t="s">
+        <v>31</v>
+      </c>
+      <c r="G123" t="s">
+        <v>178</v>
+      </c>
+      <c r="H123" t="s">
+        <v>33</v>
+      </c>
+      <c r="I123" t="s">
+        <v>34</v>
+      </c>
+      <c r="J123" t="s">
+        <v>203</v>
+      </c>
+      <c r="K123" t="s">
+        <v>36</v>
+      </c>
+      <c r="L123" t="s">
+        <v>30</v>
+      </c>
+      <c r="M123" t="s">
+        <v>160</v>
+      </c>
+      <c r="N123" t="n">
+        <v>6</v>
+      </c>
+      <c r="O123" t="n">
+        <v>0.00121326309654557</v>
+      </c>
+      <c r="P123" t="n">
+        <v>0.001203183844685555</v>
+      </c>
+      <c r="Q123" t="n">
+        <v>0.5053425936442943</v>
+      </c>
+      <c r="R123" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="S123" t="n">
+        <v>0.9370445903807563</v>
+      </c>
+      <c r="T123" t="n">
+        <v>0.8933084573650918</v>
+      </c>
+      <c r="U123" t="n">
+        <v>6</v>
+      </c>
+      <c r="V123" t="n">
+        <v>0.5053425936442943</v>
+      </c>
+      <c r="W123" t="n">
+        <v>0.503</v>
+      </c>
+      <c r="X123" t="n">
+        <v>0.9370445903807563</v>
+      </c>
+      <c r="Y123" t="n">
+        <v>0.8933084573650918</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>

</xml_diff>

<commit_message>
Dataset pruned, new results added
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -215,6 +215,156 @@
   </si>
   <si>
     <t>0.5xsingle + 0.5Xmulti</t>
+  </si>
+  <si>
+    <t>October31  14:51:35</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fbb563eeae8&gt;</t>
+  </si>
+  <si>
+    <t>October31  14:52:41</t>
+  </si>
+  <si>
+    <t>October31  14:54:58</t>
+  </si>
+  <si>
+    <t>resnet18</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7fbb563ee9d8&gt;</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>October31  14:55:19</t>
+  </si>
+  <si>
+    <t>October31  15:00:45</t>
+  </si>
+  <si>
+    <t>October31  15:01:05</t>
+  </si>
+  <si>
+    <t>October31  15:12:03</t>
+  </si>
+  <si>
+    <t>October31  15:22:59</t>
+  </si>
+  <si>
+    <t>October31  15:34:11</t>
+  </si>
+  <si>
+    <t>October31  15:45:13</t>
+  </si>
+  <si>
+    <t>October31  20:22:48</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f5d5d4a0ae8&gt;</t>
+  </si>
+  <si>
+    <t>October31  20:31:59</t>
+  </si>
+  <si>
+    <t>October31  20:41:18</t>
+  </si>
+  <si>
+    <t>October31  20:50:24</t>
+  </si>
+  <si>
+    <t>October31  20:59:21</t>
+  </si>
+  <si>
+    <t>October31  22:13:05</t>
+  </si>
+  <si>
+    <t>October31  22:21:50</t>
+  </si>
+  <si>
+    <t>October31  22:30:46</t>
+  </si>
+  <si>
+    <t>October31  22:39:47</t>
+  </si>
+  <si>
+    <t>October31  22:48:44</t>
+  </si>
+  <si>
+    <t>November01  17:42:51</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f432662aae8&gt;</t>
+  </si>
+  <si>
+    <t>November01  17:51:37</t>
+  </si>
+  <si>
+    <t>November01  18:00:01</t>
+  </si>
+  <si>
+    <t>0.3xsingle + 0.7Xmulti</t>
+  </si>
+  <si>
+    <t>November01  18:08:25</t>
+  </si>
+  <si>
+    <t>0.1xsingle + 0.9Xmulti</t>
+  </si>
+  <si>
+    <t>November01  18:16:51</t>
+  </si>
+  <si>
+    <t>November01  19:38:00</t>
+  </si>
+  <si>
+    <t>November01  19:46:14</t>
+  </si>
+  <si>
+    <t>November01  19:54:43</t>
+  </si>
+  <si>
+    <t>November01  20:03:15</t>
+  </si>
+  <si>
+    <t>November01  20:11:37</t>
+  </si>
+  <si>
+    <t>November01  20:20:04</t>
+  </si>
+  <si>
+    <t>November01  20:28:31</t>
+  </si>
+  <si>
+    <t>November01  20:37:07</t>
+  </si>
+  <si>
+    <t>November01  20:45:43</t>
+  </si>
+  <si>
+    <t>November01  20:54:12</t>
+  </si>
+  <si>
+    <t>November01  21:02:46</t>
+  </si>
+  <si>
+    <t>November01  21:08:52</t>
+  </si>
+  <si>
+    <t>November01  21:17:26</t>
+  </si>
+  <si>
+    <t>November01  21:26:05</t>
+  </si>
+  <si>
+    <t>November01  21:34:33</t>
+  </si>
+  <si>
+    <t>November01  21:43:05</t>
   </si>
 </sst>
 </file>
@@ -592,7 +742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y59"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A182" activeCellId="0" pane="topLeft" sqref="2:182"/>
@@ -1829,6 +1979,3031 @@
         <v>0.8692197847668754</v>
       </c>
     </row>
+    <row r="19" spans="1:25">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+      <c r="M19" t="s">
+        <v>36</v>
+      </c>
+      <c r="S19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M20" t="s">
+        <v>36</v>
+      </c>
+      <c r="S20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>39</v>
+      </c>
+      <c r="H21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" t="s">
+        <v>73</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" t="s">
+        <v>74</v>
+      </c>
+      <c r="N22" t="n">
+        <v>17</v>
+      </c>
+      <c r="O22" t="n">
+        <v>0.005454851099162753</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.0791793954372406</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.9522445081184336</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0.3708582163292478</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1.48492424049175</v>
+      </c>
+      <c r="U22" t="n">
+        <v>17</v>
+      </c>
+      <c r="V22" t="n">
+        <v>0.9522445081184336</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0.3708582163292478</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>1.48492424049175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" t="s">
+        <v>74</v>
+      </c>
+      <c r="S23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" t="s">
+        <v>39</v>
+      </c>
+      <c r="H24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" t="s">
+        <v>73</v>
+      </c>
+      <c r="K24" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>74</v>
+      </c>
+      <c r="N24" t="n">
+        <v>30</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0.002733449945306368</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0.07747403383255005</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.9761222540592168</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0.2529671107501901</v>
+      </c>
+      <c r="T24" t="n">
+        <v>1.473091986265624</v>
+      </c>
+      <c r="U24" t="n">
+        <v>30</v>
+      </c>
+      <c r="V24" t="n">
+        <v>0.9761222540592168</v>
+      </c>
+      <c r="W24" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.2529671107501901</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>1.473091986265624</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
+        <v>73</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" t="s">
+        <v>74</v>
+      </c>
+      <c r="N25" t="n">
+        <v>57</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0.003669285230559173</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.01426821559667587</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.612225405921681</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0.6599470326926892</v>
+      </c>
+      <c r="T25" t="n">
+        <v>1.262933094031509</v>
+      </c>
+      <c r="U25" t="n">
+        <v>57</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.612225405921681</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.6599470326926892</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>1.262933094031509</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" t="s">
+        <v>74</v>
+      </c>
+      <c r="N26" t="n">
+        <v>7</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.009149082666823379</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.0180771204829216</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.6657115568290354</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0.7963623121338689</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1.274754878398196</v>
+      </c>
+      <c r="U26" t="n">
+        <v>7</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.6657115568290354</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.7963623121338689</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>1.274754878398196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" t="s">
+        <v>62</v>
+      </c>
+      <c r="H27" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" t="s">
+        <v>73</v>
+      </c>
+      <c r="K27" t="s">
+        <v>35</v>
+      </c>
+      <c r="L27" t="s">
+        <v>29</v>
+      </c>
+      <c r="M27" t="s">
+        <v>74</v>
+      </c>
+      <c r="N27" t="n">
+        <v>35</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.003205093991904454</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.03028415113687515</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.9694364851957975</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.445</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0.2433450429598727</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1.244989959798873</v>
+      </c>
+      <c r="U27" t="n">
+        <v>35</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.9694364851957975</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.445</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.2433450429598727</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>1.244989959798873</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25">
+      <c r="A28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" t="s">
+        <v>73</v>
+      </c>
+      <c r="K28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L28" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28" t="s">
+        <v>74</v>
+      </c>
+      <c r="N28" t="n">
+        <v>41</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.003188726076822454</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.03957727819681168</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.9799426934097422</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0.2002863279919919</v>
+      </c>
+      <c r="T28" t="n">
+        <v>1.380217374184226</v>
+      </c>
+      <c r="U28" t="n">
+        <v>41</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.9799426934097422</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.455</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.2002863279919919</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>1.380217374184226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" t="s">
+        <v>32</v>
+      </c>
+      <c r="I29" t="s">
+        <v>33</v>
+      </c>
+      <c r="J29" t="s">
+        <v>83</v>
+      </c>
+      <c r="K29" t="s">
+        <v>35</v>
+      </c>
+      <c r="L29" t="s">
+        <v>29</v>
+      </c>
+      <c r="M29" t="s">
+        <v>74</v>
+      </c>
+      <c r="N29" t="n">
+        <v>29</v>
+      </c>
+      <c r="O29" t="n">
+        <v>0.006794408827150661</v>
+      </c>
+      <c r="P29" t="n">
+        <v>0.07604332500033908</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.9189627228525121</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.4222222222222222</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0.4105575921436294</v>
+      </c>
+      <c r="T29" t="n">
+        <v>1.334998959633386</v>
+      </c>
+      <c r="U29" t="n">
+        <v>29</v>
+      </c>
+      <c r="V29" t="n">
+        <v>0.9189627228525121</v>
+      </c>
+      <c r="W29" t="n">
+        <v>0.4222222222222222</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0.4105575921436294</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>1.334998959633386</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" t="s">
+        <v>33</v>
+      </c>
+      <c r="J30" t="s">
+        <v>83</v>
+      </c>
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" t="s">
+        <v>29</v>
+      </c>
+      <c r="M30" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" t="n">
+        <v>24</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.003739707455691101</v>
+      </c>
+      <c r="P30" t="n">
+        <v>0.012810653862026</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.600486223662885</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.3733333333333334</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.6485240692491389</v>
+      </c>
+      <c r="T30" t="n">
+        <v>1.271918935222594</v>
+      </c>
+      <c r="U30" t="n">
+        <v>24</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0.600486223662885</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0.3733333333333334</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0.6485240692491389</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>1.271918935222594</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" t="s">
+        <v>33</v>
+      </c>
+      <c r="J31" t="s">
+        <v>83</v>
+      </c>
+      <c r="K31" t="s">
+        <v>35</v>
+      </c>
+      <c r="L31" t="s">
+        <v>29</v>
+      </c>
+      <c r="M31" t="s">
+        <v>74</v>
+      </c>
+      <c r="N31" t="n">
+        <v>33</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.004333783695821438</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.01839789297845628</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.8606158833063209</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.4488888888888889</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.4473947636643672</v>
+      </c>
+      <c r="T31" t="n">
+        <v>1.24186240067981</v>
+      </c>
+      <c r="U31" t="n">
+        <v>33</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.8606158833063209</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.4488888888888889</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.4473947636643672</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>1.24186240067981</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" t="s">
+        <v>32</v>
+      </c>
+      <c r="I32" t="s">
+        <v>33</v>
+      </c>
+      <c r="J32" t="s">
+        <v>83</v>
+      </c>
+      <c r="K32" t="s">
+        <v>35</v>
+      </c>
+      <c r="L32" t="s">
+        <v>29</v>
+      </c>
+      <c r="M32" t="s">
+        <v>74</v>
+      </c>
+      <c r="N32" t="n">
+        <v>46</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.004933890245094098</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.03018448339568244</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.9124797406807131</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.3871937018119646</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1.308094458023239</v>
+      </c>
+      <c r="U32" t="n">
+        <v>46</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.9124797406807131</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.3871937018119646</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1.308094458023239</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" t="s">
+        <v>33</v>
+      </c>
+      <c r="J33" t="s">
+        <v>83</v>
+      </c>
+      <c r="K33" t="s">
+        <v>35</v>
+      </c>
+      <c r="L33" t="s">
+        <v>29</v>
+      </c>
+      <c r="M33" t="s">
+        <v>74</v>
+      </c>
+      <c r="N33" t="n">
+        <v>20</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.005610140454102567</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.03918958465258281</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.9278768233387358</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.4311111111111111</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.4464881877304483</v>
+      </c>
+      <c r="T33" t="n">
+        <v>1.359738536958076</v>
+      </c>
+      <c r="U33" t="n">
+        <v>20</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.9278768233387358</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.4311111111111111</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.4464881877304483</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>1.359738536958076</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" t="s">
+        <v>83</v>
+      </c>
+      <c r="K34" t="s">
+        <v>35</v>
+      </c>
+      <c r="L34" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" t="s">
+        <v>74</v>
+      </c>
+      <c r="N34" t="n">
+        <v>15</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.009099722125928252</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.07260268873638577</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.906807131280389</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.4527961033215108</v>
+      </c>
+      <c r="T34" t="n">
+        <v>1.331665623695879</v>
+      </c>
+      <c r="U34" t="n">
+        <v>15</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.906807131280389</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.4527961033215108</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>1.331665623695879</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I35" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" t="s">
+        <v>83</v>
+      </c>
+      <c r="K35" t="s">
+        <v>35</v>
+      </c>
+      <c r="L35" t="s">
+        <v>29</v>
+      </c>
+      <c r="M35" t="s">
+        <v>74</v>
+      </c>
+      <c r="N35" t="n">
+        <v>46</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.003828151697954057</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.01311924801932441</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.6247974068071313</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.3688888888888889</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.6553606403207973</v>
+      </c>
+      <c r="T35" t="n">
+        <v>1.277149604044534</v>
+      </c>
+      <c r="U35" t="n">
+        <v>46</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.6247974068071313</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.3688888888888889</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.6553606403207973</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>1.277149604044534</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H36" t="s">
+        <v>32</v>
+      </c>
+      <c r="I36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36" t="s">
+        <v>35</v>
+      </c>
+      <c r="L36" t="s">
+        <v>29</v>
+      </c>
+      <c r="M36" t="s">
+        <v>74</v>
+      </c>
+      <c r="N36" t="n">
+        <v>6</v>
+      </c>
+      <c r="O36" t="n">
+        <v>0.009886540726092878</v>
+      </c>
+      <c r="P36" t="n">
+        <v>0.01649441050158607</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.6280388978930308</v>
+      </c>
+      <c r="R36" t="n">
+        <v>0.4488888888888889</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0.8648549404792186</v>
+      </c>
+      <c r="T36" t="n">
+        <v>1.21472447721924</v>
+      </c>
+      <c r="U36" t="n">
+        <v>6</v>
+      </c>
+      <c r="V36" t="n">
+        <v>0.6280388978930308</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0.4488888888888889</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0.8648549404792186</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>1.21472447721924</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" t="s">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>62</v>
+      </c>
+      <c r="H37" t="s">
+        <v>32</v>
+      </c>
+      <c r="I37" t="s">
+        <v>33</v>
+      </c>
+      <c r="J37" t="s">
+        <v>83</v>
+      </c>
+      <c r="K37" t="s">
+        <v>35</v>
+      </c>
+      <c r="L37" t="s">
+        <v>29</v>
+      </c>
+      <c r="M37" t="s">
+        <v>74</v>
+      </c>
+      <c r="N37" t="n">
+        <v>42</v>
+      </c>
+      <c r="O37" t="n">
+        <v>0.004720399147156185</v>
+      </c>
+      <c r="P37" t="n">
+        <v>0.02778150081634521</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.9246353322528363</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="S37" t="n">
+        <v>0.3144288124837404</v>
+      </c>
+      <c r="T37" t="n">
+        <v>1.257864150940881</v>
+      </c>
+      <c r="U37" t="n">
+        <v>42</v>
+      </c>
+      <c r="V37" t="n">
+        <v>0.9246353322528363</v>
+      </c>
+      <c r="W37" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="X37" t="n">
+        <v>0.3144288124837404</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>1.257864150940881</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25">
+      <c r="A38" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>66</v>
+      </c>
+      <c r="H38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" t="s">
+        <v>83</v>
+      </c>
+      <c r="K38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L38" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38" t="s">
+        <v>74</v>
+      </c>
+      <c r="N38" t="n">
+        <v>29</v>
+      </c>
+      <c r="O38" t="n">
+        <v>0.005081898612807984</v>
+      </c>
+      <c r="P38" t="n">
+        <v>0.04848555697335137</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.9440842787682334</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0.4133333333333333</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0.3208073284345443</v>
+      </c>
+      <c r="T38" t="n">
+        <v>1.344949400122134</v>
+      </c>
+      <c r="U38" t="n">
+        <v>29</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0.9440842787682334</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0.4133333333333333</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0.3208073284345443</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>1.344949400122134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" t="s">
+        <v>30</v>
+      </c>
+      <c r="G39" t="s">
+        <v>39</v>
+      </c>
+      <c r="H39" t="s">
+        <v>32</v>
+      </c>
+      <c r="I39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J39" t="s">
+        <v>94</v>
+      </c>
+      <c r="K39" t="s">
+        <v>35</v>
+      </c>
+      <c r="L39" t="s">
+        <v>29</v>
+      </c>
+      <c r="M39" t="s">
+        <v>74</v>
+      </c>
+      <c r="N39" t="n">
+        <v>48</v>
+      </c>
+      <c r="O39" t="n">
+        <v>0.003604024330834074</v>
+      </c>
+      <c r="P39" t="n">
+        <v>0.08685855600568983</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.9652777777777778</v>
+      </c>
+      <c r="R39" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0.3753305421532011</v>
+      </c>
+      <c r="T39" t="n">
+        <v>1.61245154965971</v>
+      </c>
+      <c r="U39" t="n">
+        <v>48</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0.9652777777777778</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0.3753305421532011</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>1.61245154965971</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" t="s">
+        <v>32</v>
+      </c>
+      <c r="I40" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" t="s">
+        <v>94</v>
+      </c>
+      <c r="K40" t="s">
+        <v>35</v>
+      </c>
+      <c r="L40" t="s">
+        <v>29</v>
+      </c>
+      <c r="M40" t="s">
+        <v>74</v>
+      </c>
+      <c r="N40" t="n">
+        <v>16</v>
+      </c>
+      <c r="O40" t="n">
+        <v>0.003954248905684504</v>
+      </c>
+      <c r="P40" t="n">
+        <v>0.0564760246541765</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.9692460317460317</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0.3644444444444445</v>
+      </c>
+      <c r="S40" t="n">
+        <v>0.263523138347365</v>
+      </c>
+      <c r="T40" t="n">
+        <v>1.477234653744023</v>
+      </c>
+      <c r="U40" t="n">
+        <v>16</v>
+      </c>
+      <c r="V40" t="n">
+        <v>0.9692460317460317</v>
+      </c>
+      <c r="W40" t="n">
+        <v>0.3644444444444445</v>
+      </c>
+      <c r="X40" t="n">
+        <v>0.263523138347365</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>1.477234653744023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41" t="s">
+        <v>29</v>
+      </c>
+      <c r="F41" t="s">
+        <v>30</v>
+      </c>
+      <c r="G41" t="s">
+        <v>97</v>
+      </c>
+      <c r="H41" t="s">
+        <v>32</v>
+      </c>
+      <c r="I41" t="s">
+        <v>33</v>
+      </c>
+      <c r="J41" t="s">
+        <v>94</v>
+      </c>
+      <c r="K41" t="s">
+        <v>35</v>
+      </c>
+      <c r="L41" t="s">
+        <v>29</v>
+      </c>
+      <c r="M41" t="s">
+        <v>74</v>
+      </c>
+      <c r="N41" t="n">
+        <v>12</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0.005497866709317479</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0.03996873829099867</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.9305555555555556</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0.3733333333333334</v>
+      </c>
+      <c r="S41" t="n">
+        <v>0.4106711502538176</v>
+      </c>
+      <c r="T41" t="n">
+        <v>1.319932658214889</v>
+      </c>
+      <c r="U41" t="n">
+        <v>12</v>
+      </c>
+      <c r="V41" t="n">
+        <v>0.9305555555555556</v>
+      </c>
+      <c r="W41" t="n">
+        <v>0.3733333333333334</v>
+      </c>
+      <c r="X41" t="n">
+        <v>0.4106711502538176</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>1.319932658214889</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>28</v>
+      </c>
+      <c r="E42" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" t="s">
+        <v>30</v>
+      </c>
+      <c r="G42" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" t="s">
+        <v>32</v>
+      </c>
+      <c r="I42" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" t="s">
+        <v>94</v>
+      </c>
+      <c r="K42" t="s">
+        <v>35</v>
+      </c>
+      <c r="L42" t="s">
+        <v>29</v>
+      </c>
+      <c r="M42" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42" t="n">
+        <v>30</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0.003841723603684278</v>
+      </c>
+      <c r="P42" t="n">
+        <v>0.02492503596676721</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.8849206349206349</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="S42" t="n">
+        <v>0.3713446181067196</v>
+      </c>
+      <c r="T42" t="n">
+        <v>1.449904211395436</v>
+      </c>
+      <c r="U42" t="n">
+        <v>30</v>
+      </c>
+      <c r="V42" t="n">
+        <v>0.8849206349206349</v>
+      </c>
+      <c r="W42" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X42" t="n">
+        <v>0.3713446181067196</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>1.449904211395436</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25">
+      <c r="A43" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>31</v>
+      </c>
+      <c r="H43" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" t="s">
+        <v>33</v>
+      </c>
+      <c r="J43" t="s">
+        <v>94</v>
+      </c>
+      <c r="K43" t="s">
+        <v>35</v>
+      </c>
+      <c r="L43" t="s">
+        <v>29</v>
+      </c>
+      <c r="M43" t="s">
+        <v>74</v>
+      </c>
+      <c r="N43" t="n">
+        <v>21</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0.003657553507576859</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0.01714543965127733</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.5952380952380952</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="S43" t="n">
+        <v>0.7064049380546094</v>
+      </c>
+      <c r="T43" t="n">
+        <v>1.361371857110809</v>
+      </c>
+      <c r="U43" t="n">
+        <v>21</v>
+      </c>
+      <c r="V43" t="n">
+        <v>0.5952380952380952</v>
+      </c>
+      <c r="W43" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="X43" t="n">
+        <v>0.7064049380546094</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>1.361371857110809</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25">
+      <c r="A44" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" t="s">
+        <v>30</v>
+      </c>
+      <c r="G44" t="s">
+        <v>39</v>
+      </c>
+      <c r="H44" t="s">
+        <v>32</v>
+      </c>
+      <c r="I44" t="s">
+        <v>33</v>
+      </c>
+      <c r="J44" t="s">
+        <v>94</v>
+      </c>
+      <c r="K44" t="s">
+        <v>35</v>
+      </c>
+      <c r="L44" t="s">
+        <v>29</v>
+      </c>
+      <c r="M44" t="s">
+        <v>74</v>
+      </c>
+      <c r="N44" t="n">
+        <v>17</v>
+      </c>
+      <c r="O44" t="n">
+        <v>0.005419946216519863</v>
+      </c>
+      <c r="P44" t="n">
+        <v>0.1076946510208978</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.9553571428571429</v>
+      </c>
+      <c r="R44" t="n">
+        <v>0.3822222222222222</v>
+      </c>
+      <c r="S44" t="n">
+        <v>0.4070314523161609</v>
+      </c>
+      <c r="T44" t="n">
+        <v>1.581841402360623</v>
+      </c>
+      <c r="U44" t="n">
+        <v>17</v>
+      </c>
+      <c r="V44" t="n">
+        <v>0.9553571428571429</v>
+      </c>
+      <c r="W44" t="n">
+        <v>0.3822222222222222</v>
+      </c>
+      <c r="X44" t="n">
+        <v>0.4070314523161609</v>
+      </c>
+      <c r="Y44" t="n">
+        <v>1.581841402360623</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25">
+      <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" t="s">
+        <v>30</v>
+      </c>
+      <c r="G45" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" t="s">
+        <v>32</v>
+      </c>
+      <c r="I45" t="s">
+        <v>33</v>
+      </c>
+      <c r="J45" t="s">
+        <v>94</v>
+      </c>
+      <c r="K45" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" t="s">
+        <v>29</v>
+      </c>
+      <c r="M45" t="s">
+        <v>74</v>
+      </c>
+      <c r="N45" t="n">
+        <v>18</v>
+      </c>
+      <c r="O45" t="n">
+        <v>0.00385495253084671</v>
+      </c>
+      <c r="P45" t="n">
+        <v>0.04872551434569888</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>0.9732142857142857</v>
+      </c>
+      <c r="R45" t="n">
+        <v>0.3911111111111111</v>
+      </c>
+      <c r="S45" t="n">
+        <v>0.2653987715429518</v>
+      </c>
+      <c r="T45" t="n">
+        <v>1.406334873981932</v>
+      </c>
+      <c r="U45" t="n">
+        <v>18</v>
+      </c>
+      <c r="V45" t="n">
+        <v>0.9732142857142857</v>
+      </c>
+      <c r="W45" t="n">
+        <v>0.3911111111111111</v>
+      </c>
+      <c r="X45" t="n">
+        <v>0.2653987715429518</v>
+      </c>
+      <c r="Y45" t="n">
+        <v>1.406334873981932</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25">
+      <c r="A46" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G46" t="s">
+        <v>97</v>
+      </c>
+      <c r="H46" t="s">
+        <v>32</v>
+      </c>
+      <c r="I46" t="s">
+        <v>33</v>
+      </c>
+      <c r="J46" t="s">
+        <v>94</v>
+      </c>
+      <c r="K46" t="s">
+        <v>35</v>
+      </c>
+      <c r="L46" t="s">
+        <v>29</v>
+      </c>
+      <c r="M46" t="s">
+        <v>74</v>
+      </c>
+      <c r="N46" t="n">
+        <v>3</v>
+      </c>
+      <c r="O46" t="n">
+        <v>0.01887778390849394</v>
+      </c>
+      <c r="P46" t="n">
+        <v>0.03131733218828837</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.5396825396825397</v>
+      </c>
+      <c r="R46" t="n">
+        <v>0.3822222222222222</v>
+      </c>
+      <c r="S46" t="n">
+        <v>1.15298095360031</v>
+      </c>
+      <c r="T46" t="n">
+        <v>1.41578403877302</v>
+      </c>
+      <c r="U46" t="n">
+        <v>3</v>
+      </c>
+      <c r="V46" t="n">
+        <v>0.5396825396825397</v>
+      </c>
+      <c r="W46" t="n">
+        <v>0.3822222222222222</v>
+      </c>
+      <c r="X46" t="n">
+        <v>1.15298095360031</v>
+      </c>
+      <c r="Y46" t="n">
+        <v>1.41578403877302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25">
+      <c r="A47" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+      <c r="F47" t="s">
+        <v>30</v>
+      </c>
+      <c r="G47" t="s">
+        <v>99</v>
+      </c>
+      <c r="H47" t="s">
+        <v>32</v>
+      </c>
+      <c r="I47" t="s">
+        <v>33</v>
+      </c>
+      <c r="J47" t="s">
+        <v>94</v>
+      </c>
+      <c r="K47" t="s">
+        <v>35</v>
+      </c>
+      <c r="L47" t="s">
+        <v>29</v>
+      </c>
+      <c r="M47" t="s">
+        <v>74</v>
+      </c>
+      <c r="N47" t="n">
+        <v>44</v>
+      </c>
+      <c r="O47" t="n">
+        <v>0.003940228616730088</v>
+      </c>
+      <c r="P47" t="n">
+        <v>0.02305696805318197</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.9007936507936508</v>
+      </c>
+      <c r="R47" t="n">
+        <v>0.4355555555555555</v>
+      </c>
+      <c r="S47" t="n">
+        <v>0.4021272798584414</v>
+      </c>
+      <c r="T47" t="n">
+        <v>1.309792180292567</v>
+      </c>
+      <c r="U47" t="n">
+        <v>44</v>
+      </c>
+      <c r="V47" t="n">
+        <v>0.9007936507936508</v>
+      </c>
+      <c r="W47" t="n">
+        <v>0.4355555555555555</v>
+      </c>
+      <c r="X47" t="n">
+        <v>0.4021272798584414</v>
+      </c>
+      <c r="Y47" t="n">
+        <v>1.309792180292567</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25">
+      <c r="A48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" t="s">
+        <v>72</v>
+      </c>
+      <c r="D48" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" t="s">
+        <v>29</v>
+      </c>
+      <c r="F48" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" t="s">
+        <v>31</v>
+      </c>
+      <c r="H48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I48" t="s">
+        <v>33</v>
+      </c>
+      <c r="J48" t="s">
+        <v>94</v>
+      </c>
+      <c r="K48" t="s">
+        <v>35</v>
+      </c>
+      <c r="L48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M48" t="s">
+        <v>74</v>
+      </c>
+      <c r="N48" t="n">
+        <v>5</v>
+      </c>
+      <c r="O48" t="n">
+        <v>0.009201027585991792</v>
+      </c>
+      <c r="P48" t="n">
+        <v>0.01485018369224336</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.3938492063492063</v>
+      </c>
+      <c r="R48" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+      <c r="S48" t="n">
+        <v>1.055973183882699</v>
+      </c>
+      <c r="T48" t="n">
+        <v>1.417352775031287</v>
+      </c>
+      <c r="U48" t="n">
+        <v>5</v>
+      </c>
+      <c r="V48" t="n">
+        <v>0.3938492063492063</v>
+      </c>
+      <c r="W48" t="n">
+        <v>0.2666666666666667</v>
+      </c>
+      <c r="X48" t="n">
+        <v>1.055973183882699</v>
+      </c>
+      <c r="Y48" t="n">
+        <v>1.417352775031287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25">
+      <c r="A49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" t="s">
+        <v>29</v>
+      </c>
+      <c r="F49" t="s">
+        <v>30</v>
+      </c>
+      <c r="G49" t="s">
+        <v>39</v>
+      </c>
+      <c r="H49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I49" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" t="s">
+        <v>94</v>
+      </c>
+      <c r="K49" t="s">
+        <v>35</v>
+      </c>
+      <c r="L49" t="s">
+        <v>29</v>
+      </c>
+      <c r="M49" t="s">
+        <v>74</v>
+      </c>
+      <c r="N49" t="n">
+        <v>19</v>
+      </c>
+      <c r="O49" t="n">
+        <v>0.004169532637451849</v>
+      </c>
+      <c r="P49" t="n">
+        <v>0.09957129769855075</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="R49" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="S49" t="n">
+        <v>0.3779644730092272</v>
+      </c>
+      <c r="T49" t="n">
+        <v>1.577621275493231</v>
+      </c>
+      <c r="U49" t="n">
+        <v>19</v>
+      </c>
+      <c r="V49" t="n">
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="W49" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="X49" t="n">
+        <v>0.3779644730092272</v>
+      </c>
+      <c r="Y49" t="n">
+        <v>1.577621275493231</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G50" t="s">
+        <v>66</v>
+      </c>
+      <c r="H50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I50" t="s">
+        <v>33</v>
+      </c>
+      <c r="J50" t="s">
+        <v>94</v>
+      </c>
+      <c r="K50" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" t="s">
+        <v>29</v>
+      </c>
+      <c r="M50" t="s">
+        <v>74</v>
+      </c>
+      <c r="N50" t="n">
+        <v>45</v>
+      </c>
+      <c r="O50" t="n">
+        <v>0.003177450452413824</v>
+      </c>
+      <c r="P50" t="n">
+        <v>0.05874054167005751</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>0.9831349206349206</v>
+      </c>
+      <c r="R50" t="n">
+        <v>0.3644444444444445</v>
+      </c>
+      <c r="S50" t="n">
+        <v>0.1915890111837034</v>
+      </c>
+      <c r="T50" t="n">
+        <v>1.440678852331621</v>
+      </c>
+      <c r="U50" t="n">
+        <v>45</v>
+      </c>
+      <c r="V50" t="n">
+        <v>0.9831349206349206</v>
+      </c>
+      <c r="W50" t="n">
+        <v>0.3644444444444445</v>
+      </c>
+      <c r="X50" t="n">
+        <v>0.1915890111837034</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>1.440678852331621</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" t="s">
+        <v>30</v>
+      </c>
+      <c r="G51" t="s">
+        <v>97</v>
+      </c>
+      <c r="H51" t="s">
+        <v>32</v>
+      </c>
+      <c r="I51" t="s">
+        <v>33</v>
+      </c>
+      <c r="J51" t="s">
+        <v>94</v>
+      </c>
+      <c r="K51" t="s">
+        <v>35</v>
+      </c>
+      <c r="L51" t="s">
+        <v>29</v>
+      </c>
+      <c r="M51" t="s">
+        <v>74</v>
+      </c>
+      <c r="N51" t="n">
+        <v>8</v>
+      </c>
+      <c r="O51" t="n">
+        <v>0.009517232044821694</v>
+      </c>
+      <c r="P51" t="n">
+        <v>0.04081181963284811</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>0.8035714285714286</v>
+      </c>
+      <c r="R51" t="n">
+        <v>0.4177777777777778</v>
+      </c>
+      <c r="S51" t="n">
+        <v>0.7154752000627009</v>
+      </c>
+      <c r="T51" t="n">
+        <v>1.469693845669907</v>
+      </c>
+      <c r="U51" t="n">
+        <v>8</v>
+      </c>
+      <c r="V51" t="n">
+        <v>0.8035714285714286</v>
+      </c>
+      <c r="W51" t="n">
+        <v>0.4177777777777778</v>
+      </c>
+      <c r="X51" t="n">
+        <v>0.7154752000627009</v>
+      </c>
+      <c r="Y51" t="n">
+        <v>1.469693845669907</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25">
+      <c r="A52" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" t="s">
+        <v>30</v>
+      </c>
+      <c r="G52" t="s">
+        <v>99</v>
+      </c>
+      <c r="H52" t="s">
+        <v>32</v>
+      </c>
+      <c r="I52" t="s">
+        <v>33</v>
+      </c>
+      <c r="J52" t="s">
+        <v>94</v>
+      </c>
+      <c r="K52" t="s">
+        <v>35</v>
+      </c>
+      <c r="L52" t="s">
+        <v>29</v>
+      </c>
+      <c r="M52" t="s">
+        <v>74</v>
+      </c>
+      <c r="N52" t="n">
+        <v>35</v>
+      </c>
+      <c r="O52" t="n">
+        <v>0.00378944772842621</v>
+      </c>
+      <c r="P52" t="n">
+        <v>0.02213342454698351</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.8988095238095238</v>
+      </c>
+      <c r="R52" t="n">
+        <v>0.3911111111111111</v>
+      </c>
+      <c r="S52" t="n">
+        <v>0.3659625273557</v>
+      </c>
+      <c r="T52" t="n">
+        <v>1.299572579307862</v>
+      </c>
+      <c r="U52" t="n">
+        <v>35</v>
+      </c>
+      <c r="V52" t="n">
+        <v>0.8988095238095238</v>
+      </c>
+      <c r="W52" t="n">
+        <v>0.3911111111111111</v>
+      </c>
+      <c r="X52" t="n">
+        <v>0.3659625273557</v>
+      </c>
+      <c r="Y52" t="n">
+        <v>1.299572579307862</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" t="s">
+        <v>30</v>
+      </c>
+      <c r="G53" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" t="s">
+        <v>32</v>
+      </c>
+      <c r="I53" t="s">
+        <v>33</v>
+      </c>
+      <c r="J53" t="s">
+        <v>94</v>
+      </c>
+      <c r="K53" t="s">
+        <v>35</v>
+      </c>
+      <c r="L53" t="s">
+        <v>29</v>
+      </c>
+      <c r="M53" t="s">
+        <v>74</v>
+      </c>
+      <c r="N53" t="n">
+        <v>5</v>
+      </c>
+      <c r="O53" t="n">
+        <v>0.009437856279195302</v>
+      </c>
+      <c r="P53" t="n">
+        <v>0.01571711430946986</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>0.376984126984127</v>
+      </c>
+      <c r="R53" t="n">
+        <v>0.2888888888888889</v>
+      </c>
+      <c r="S53" t="n">
+        <v>1.142174895567002</v>
+      </c>
+      <c r="T53" t="n">
+        <v>1.411067365901115</v>
+      </c>
+      <c r="U53" t="n">
+        <v>5</v>
+      </c>
+      <c r="V53" t="n">
+        <v>0.376984126984127</v>
+      </c>
+      <c r="W53" t="n">
+        <v>0.2888888888888889</v>
+      </c>
+      <c r="X53" t="n">
+        <v>1.142174895567002</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>1.411067365901115</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>71</v>
+      </c>
+      <c r="C54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" t="s">
+        <v>29</v>
+      </c>
+      <c r="F54" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" t="s">
+        <v>39</v>
+      </c>
+      <c r="H54" t="s">
+        <v>32</v>
+      </c>
+      <c r="I54" t="s">
+        <v>33</v>
+      </c>
+      <c r="J54" t="s">
+        <v>94</v>
+      </c>
+      <c r="K54" t="s">
+        <v>35</v>
+      </c>
+      <c r="L54" t="s">
+        <v>29</v>
+      </c>
+      <c r="M54" t="s">
+        <v>74</v>
+      </c>
+      <c r="N54" t="n">
+        <v>29</v>
+      </c>
+      <c r="O54" t="n">
+        <v>0.003525404747398127</v>
+      </c>
+      <c r="P54" t="n">
+        <v>0.1155569903055827</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.9692460317460317</v>
+      </c>
+      <c r="R54" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="S54" t="n">
+        <v>0.3406925719346234</v>
+      </c>
+      <c r="T54" t="n">
+        <v>1.501110699893027</v>
+      </c>
+      <c r="U54" t="n">
+        <v>29</v>
+      </c>
+      <c r="V54" t="n">
+        <v>0.9692460317460317</v>
+      </c>
+      <c r="W54" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="X54" t="n">
+        <v>0.3406925719346234</v>
+      </c>
+      <c r="Y54" t="n">
+        <v>1.501110699893027</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25">
+      <c r="A55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="G55" t="s">
+        <v>31</v>
+      </c>
+      <c r="H55" t="s">
+        <v>32</v>
+      </c>
+      <c r="I55" t="s">
+        <v>33</v>
+      </c>
+      <c r="J55" t="s">
+        <v>94</v>
+      </c>
+      <c r="K55" t="s">
+        <v>35</v>
+      </c>
+      <c r="L55" t="s">
+        <v>29</v>
+      </c>
+      <c r="M55" t="s">
+        <v>74</v>
+      </c>
+      <c r="N55" t="n">
+        <v>9</v>
+      </c>
+      <c r="O55" t="n">
+        <v>0.005777510806977275</v>
+      </c>
+      <c r="P55" t="n">
+        <v>0.01561967942449782</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>0.5188492063492064</v>
+      </c>
+      <c r="R55" t="n">
+        <v>0.3155555555555555</v>
+      </c>
+      <c r="S55" t="n">
+        <v>0.8061027151061999</v>
+      </c>
+      <c r="T55" t="n">
+        <v>1.358103252497558</v>
+      </c>
+      <c r="U55" t="n">
+        <v>9</v>
+      </c>
+      <c r="V55" t="n">
+        <v>0.5188492063492064</v>
+      </c>
+      <c r="W55" t="n">
+        <v>0.3155555555555555</v>
+      </c>
+      <c r="X55" t="n">
+        <v>0.8061027151061999</v>
+      </c>
+      <c r="Y55" t="n">
+        <v>1.358103252497558</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" t="s">
+        <v>72</v>
+      </c>
+      <c r="D56" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" t="s">
+        <v>29</v>
+      </c>
+      <c r="F56" t="s">
+        <v>30</v>
+      </c>
+      <c r="G56" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" t="s">
+        <v>32</v>
+      </c>
+      <c r="I56" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" t="s">
+        <v>94</v>
+      </c>
+      <c r="K56" t="s">
+        <v>35</v>
+      </c>
+      <c r="L56" t="s">
+        <v>29</v>
+      </c>
+      <c r="M56" t="s">
+        <v>74</v>
+      </c>
+      <c r="N56" t="n">
+        <v>17</v>
+      </c>
+      <c r="O56" t="n">
+        <v>0.004033327206141419</v>
+      </c>
+      <c r="P56" t="n">
+        <v>0.0173887801501486</v>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.6001984126984127</v>
+      </c>
+      <c r="R56" t="n">
+        <v>0.3066666666666666</v>
+      </c>
+      <c r="S56" t="n">
+        <v>0.6508541396588878</v>
+      </c>
+      <c r="T56" t="n">
+        <v>1.425170555095463</v>
+      </c>
+      <c r="U56" t="n">
+        <v>17</v>
+      </c>
+      <c r="V56" t="n">
+        <v>0.6001984126984127</v>
+      </c>
+      <c r="W56" t="n">
+        <v>0.3066666666666666</v>
+      </c>
+      <c r="X56" t="n">
+        <v>0.6508541396588878</v>
+      </c>
+      <c r="Y56" t="n">
+        <v>1.425170555095463</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>71</v>
+      </c>
+      <c r="C57" t="s">
+        <v>72</v>
+      </c>
+      <c r="D57" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F57" t="s">
+        <v>30</v>
+      </c>
+      <c r="G57" t="s">
+        <v>31</v>
+      </c>
+      <c r="H57" t="s">
+        <v>32</v>
+      </c>
+      <c r="I57" t="s">
+        <v>33</v>
+      </c>
+      <c r="J57" t="s">
+        <v>94</v>
+      </c>
+      <c r="K57" t="s">
+        <v>35</v>
+      </c>
+      <c r="L57" t="s">
+        <v>29</v>
+      </c>
+      <c r="M57" t="s">
+        <v>74</v>
+      </c>
+      <c r="N57" t="n">
+        <v>36</v>
+      </c>
+      <c r="O57" t="n">
+        <v>0.003618776820422638</v>
+      </c>
+      <c r="P57" t="n">
+        <v>0.01685757438341777</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.6140873015873016</v>
+      </c>
+      <c r="R57" t="n">
+        <v>0.2977777777777778</v>
+      </c>
+      <c r="S57" t="n">
+        <v>0.6651769068904282</v>
+      </c>
+      <c r="T57" t="n">
+        <v>1.39522996909709</v>
+      </c>
+      <c r="U57" t="n">
+        <v>36</v>
+      </c>
+      <c r="V57" t="n">
+        <v>0.6140873015873016</v>
+      </c>
+      <c r="W57" t="n">
+        <v>0.2977777777777778</v>
+      </c>
+      <c r="X57" t="n">
+        <v>0.6651769068904282</v>
+      </c>
+      <c r="Y57" t="n">
+        <v>1.39522996909709</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>72</v>
+      </c>
+      <c r="D58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" t="s">
+        <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" t="s">
+        <v>32</v>
+      </c>
+      <c r="I58" t="s">
+        <v>33</v>
+      </c>
+      <c r="J58" t="s">
+        <v>94</v>
+      </c>
+      <c r="K58" t="s">
+        <v>35</v>
+      </c>
+      <c r="L58" t="s">
+        <v>29</v>
+      </c>
+      <c r="M58" t="s">
+        <v>74</v>
+      </c>
+      <c r="N58" t="n">
+        <v>9</v>
+      </c>
+      <c r="O58" t="n">
+        <v>0.006184594676135078</v>
+      </c>
+      <c r="P58" t="n">
+        <v>0.01724316471152836</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.4880952380952381</v>
+      </c>
+      <c r="R58" t="n">
+        <v>0.2622222222222222</v>
+      </c>
+      <c r="S58" t="n">
+        <v>0.8643053913541263</v>
+      </c>
+      <c r="T58" t="n">
+        <v>1.448370732160029</v>
+      </c>
+      <c r="U58" t="n">
+        <v>9</v>
+      </c>
+      <c r="V58" t="n">
+        <v>0.4880952380952381</v>
+      </c>
+      <c r="W58" t="n">
+        <v>0.2622222222222222</v>
+      </c>
+      <c r="X58" t="n">
+        <v>0.8643053913541263</v>
+      </c>
+      <c r="Y58" t="n">
+        <v>1.448370732160029</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" t="s">
+        <v>29</v>
+      </c>
+      <c r="F59" t="s">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>31</v>
+      </c>
+      <c r="H59" t="s">
+        <v>32</v>
+      </c>
+      <c r="I59" t="s">
+        <v>33</v>
+      </c>
+      <c r="J59" t="s">
+        <v>94</v>
+      </c>
+      <c r="K59" t="s">
+        <v>35</v>
+      </c>
+      <c r="L59" t="s">
+        <v>29</v>
+      </c>
+      <c r="M59" t="s">
+        <v>74</v>
+      </c>
+      <c r="N59" t="n">
+        <v>5</v>
+      </c>
+      <c r="O59" t="n">
+        <v>0.009176860903463667</v>
+      </c>
+      <c r="P59" t="n">
+        <v>0.01418255117204454</v>
+      </c>
+      <c r="Q59" t="n">
+        <v>0.3998015873015873</v>
+      </c>
+      <c r="R59" t="n">
+        <v>0.2711111111111111</v>
+      </c>
+      <c r="S59" t="n">
+        <v>1.087902452443116</v>
+      </c>
+      <c r="T59" t="n">
+        <v>1.372750685464933</v>
+      </c>
+      <c r="U59" t="n">
+        <v>5</v>
+      </c>
+      <c r="V59" t="n">
+        <v>0.3998015873015873</v>
+      </c>
+      <c r="W59" t="n">
+        <v>0.2711111111111111</v>
+      </c>
+      <c r="X59" t="n">
+        <v>1.087902452443116</v>
+      </c>
+      <c r="Y59" t="n">
+        <v>1.372750685464933</v>
+      </c>
+    </row>
     <row customHeight="1" ht="12.8" r="1048576" s="3" spans="1:25"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>

<commit_message>
Added cross-validation code and code for generating detailed results
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
   <si>
     <t>Date</t>
   </si>
@@ -365,6 +365,78 @@
   </si>
   <si>
     <t>November01  21:43:05</t>
+  </si>
+  <si>
+    <t>November08  12:34:04</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f02f072fae8&gt;</t>
+  </si>
+  <si>
+    <t>November08  12:58:37</t>
+  </si>
+  <si>
+    <t>November08  13:00:09</t>
+  </si>
+  <si>
+    <t>November08  13:02:49</t>
+  </si>
+  <si>
+    <t>November08  13:03:49</t>
+  </si>
+  <si>
+    <t>November08  13:04:11</t>
+  </si>
+  <si>
+    <t>November08  13:04:51</t>
+  </si>
+  <si>
+    <t>November08  16:35:36</t>
+  </si>
+  <si>
+    <t>November08  16:36:05</t>
+  </si>
+  <si>
+    <t>November08  16:36:43</t>
+  </si>
+  <si>
+    <t>November08  18:07:07</t>
+  </si>
+  <si>
+    <t>November08  18:16:02</t>
+  </si>
+  <si>
+    <t>November08  18:45:25</t>
+  </si>
+  <si>
+    <t>November08  18:47:10</t>
+  </si>
+  <si>
+    <t>November08  18:48:33</t>
+  </si>
+  <si>
+    <t>November08  18:50:35</t>
+  </si>
+  <si>
+    <t>November08  18:51:13</t>
+  </si>
+  <si>
+    <t>November08  19:15:17</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f974642ca60&gt;</t>
+  </si>
+  <si>
+    <t>November08  19:15:47</t>
+  </si>
+  <si>
+    <t>November08  19:16:08</t>
+  </si>
+  <si>
+    <t>November08  19:16:29</t>
+  </si>
+  <si>
+    <t>November08  19:16:50</t>
   </si>
 </sst>
 </file>
@@ -742,7 +814,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y59"/>
+  <dimension ref="A1:Y81"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A182" activeCellId="0" pane="topLeft" sqref="2:182"/>
@@ -5004,6 +5076,1535 @@
         <v>1.372750685464933</v>
       </c>
     </row>
+    <row r="60" spans="1:25">
+      <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" t="s">
+        <v>30</v>
+      </c>
+      <c r="G60" t="s">
+        <v>39</v>
+      </c>
+      <c r="H60" t="s">
+        <v>32</v>
+      </c>
+      <c r="I60" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60" t="s">
+        <v>118</v>
+      </c>
+      <c r="K60" t="s">
+        <v>35</v>
+      </c>
+      <c r="L60" t="s">
+        <v>29</v>
+      </c>
+      <c r="M60" t="s">
+        <v>74</v>
+      </c>
+      <c r="N60" t="n">
+        <v>1</v>
+      </c>
+      <c r="O60" t="n">
+        <v>0.06318670014540355</v>
+      </c>
+      <c r="P60" t="n">
+        <v>0.08333185275395712</v>
+      </c>
+      <c r="Q60" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="R60" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="S60" t="n">
+        <v>2.167353371031276</v>
+      </c>
+      <c r="T60" t="n">
+        <v>1.70749979664876</v>
+      </c>
+      <c r="U60" t="n">
+        <v>1</v>
+      </c>
+      <c r="V60" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+      <c r="W60" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="X60" t="n">
+        <v>2.167353371031276</v>
+      </c>
+      <c r="Y60" t="n">
+        <v>1.70749979664876</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
+      <c r="A61" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" t="s">
+        <v>39</v>
+      </c>
+      <c r="H61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" t="s">
+        <v>33</v>
+      </c>
+      <c r="J61" t="s">
+        <v>118</v>
+      </c>
+      <c r="K61" t="s">
+        <v>35</v>
+      </c>
+      <c r="L61" t="s">
+        <v>29</v>
+      </c>
+      <c r="M61" t="s">
+        <v>74</v>
+      </c>
+      <c r="N61" t="n">
+        <v>1</v>
+      </c>
+      <c r="O61" t="n">
+        <v>0.06463994381446687</v>
+      </c>
+      <c r="P61" t="n">
+        <v>0.07156804349687364</v>
+      </c>
+      <c r="Q61" t="n">
+        <v>0.248015873015873</v>
+      </c>
+      <c r="R61" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="S61" t="n">
+        <v>2.188760974426994</v>
+      </c>
+      <c r="T61" t="n">
+        <v>1.742284579382931</v>
+      </c>
+      <c r="U61" t="n">
+        <v>1</v>
+      </c>
+      <c r="V61" t="n">
+        <v>0.248015873015873</v>
+      </c>
+      <c r="W61" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="X61" t="n">
+        <v>2.188760974426994</v>
+      </c>
+      <c r="Y61" t="n">
+        <v>1.742284579382931</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
+      <c r="A62" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+      <c r="D62" t="s">
+        <v>28</v>
+      </c>
+      <c r="E62" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" t="s">
+        <v>30</v>
+      </c>
+      <c r="G62" t="s">
+        <v>39</v>
+      </c>
+      <c r="H62" t="s">
+        <v>32</v>
+      </c>
+      <c r="I62" t="s">
+        <v>33</v>
+      </c>
+      <c r="J62" t="s">
+        <v>118</v>
+      </c>
+      <c r="K62" t="s">
+        <v>35</v>
+      </c>
+      <c r="L62" t="s">
+        <v>29</v>
+      </c>
+      <c r="M62" t="s">
+        <v>74</v>
+      </c>
+      <c r="N62" t="n">
+        <v>3</v>
+      </c>
+      <c r="O62" t="n">
+        <v>0.05018508398816699</v>
+      </c>
+      <c r="P62" t="n">
+        <v>0.07594142463472155</v>
+      </c>
+      <c r="Q62" t="n">
+        <v>0.4474206349206349</v>
+      </c>
+      <c r="R62" t="n">
+        <v>0.3377777777777778</v>
+      </c>
+      <c r="S62" t="n">
+        <v>1.569172261831564</v>
+      </c>
+      <c r="T62" t="n">
+        <v>2.092313976863362</v>
+      </c>
+      <c r="U62" t="n">
+        <v>3</v>
+      </c>
+      <c r="V62" t="n">
+        <v>0.4474206349206349</v>
+      </c>
+      <c r="W62" t="n">
+        <v>0.3377777777777778</v>
+      </c>
+      <c r="X62" t="n">
+        <v>1.569172261831564</v>
+      </c>
+      <c r="Y62" t="n">
+        <v>2.092313976863362</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
+      <c r="A63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" t="s">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+      <c r="D63" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F63" t="s">
+        <v>30</v>
+      </c>
+      <c r="G63" t="s">
+        <v>39</v>
+      </c>
+      <c r="H63" t="s">
+        <v>32</v>
+      </c>
+      <c r="I63" t="s">
+        <v>33</v>
+      </c>
+      <c r="J63" t="s">
+        <v>118</v>
+      </c>
+      <c r="K63" t="s">
+        <v>35</v>
+      </c>
+      <c r="L63" t="s">
+        <v>29</v>
+      </c>
+      <c r="M63" t="s">
+        <v>74</v>
+      </c>
+      <c r="N63" t="n">
+        <v>1</v>
+      </c>
+      <c r="O63" t="n">
+        <v>0.06712434795640763</v>
+      </c>
+      <c r="P63" t="n">
+        <v>0.1484774870342679</v>
+      </c>
+      <c r="Q63" t="n">
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="R63" t="n">
+        <v>0.2088888888888889</v>
+      </c>
+      <c r="S63" t="n">
+        <v>2.342033101307291</v>
+      </c>
+      <c r="T63" t="n">
+        <v>2.318045153428494</v>
+      </c>
+      <c r="U63" t="n">
+        <v>1</v>
+      </c>
+      <c r="V63" t="n">
+        <v>0.2361111111111111</v>
+      </c>
+      <c r="W63" t="n">
+        <v>0.2088888888888889</v>
+      </c>
+      <c r="X63" t="n">
+        <v>2.342033101307291</v>
+      </c>
+      <c r="Y63" t="n">
+        <v>2.318045153428494</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25">
+      <c r="A64" t="s">
+        <v>122</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" t="s">
+        <v>29</v>
+      </c>
+      <c r="F64" t="s">
+        <v>30</v>
+      </c>
+      <c r="G64" t="s">
+        <v>39</v>
+      </c>
+      <c r="H64" t="s">
+        <v>32</v>
+      </c>
+      <c r="I64" t="s">
+        <v>33</v>
+      </c>
+      <c r="J64" t="s">
+        <v>118</v>
+      </c>
+      <c r="K64" t="s">
+        <v>35</v>
+      </c>
+      <c r="L64" t="s">
+        <v>29</v>
+      </c>
+      <c r="M64" t="s">
+        <v>74</v>
+      </c>
+      <c r="S64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25">
+      <c r="A65" t="s">
+        <v>123</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F65" t="s">
+        <v>30</v>
+      </c>
+      <c r="G65" t="s">
+        <v>39</v>
+      </c>
+      <c r="H65" t="s">
+        <v>32</v>
+      </c>
+      <c r="I65" t="s">
+        <v>33</v>
+      </c>
+      <c r="J65" t="s">
+        <v>118</v>
+      </c>
+      <c r="K65" t="s">
+        <v>35</v>
+      </c>
+      <c r="L65" t="s">
+        <v>29</v>
+      </c>
+      <c r="M65" t="s">
+        <v>74</v>
+      </c>
+      <c r="N65" t="n">
+        <v>1</v>
+      </c>
+      <c r="O65" t="n">
+        <v>0.06717570610935726</v>
+      </c>
+      <c r="P65" t="n">
+        <v>0.08469244215223524</v>
+      </c>
+      <c r="Q65" t="n">
+        <v>0.244047619047619</v>
+      </c>
+      <c r="R65" t="n">
+        <v>0.2888888888888889</v>
+      </c>
+      <c r="S65" t="n">
+        <v>2.251542681017716</v>
+      </c>
+      <c r="T65" t="n">
+        <v>1.967513941783161</v>
+      </c>
+      <c r="U65" t="n">
+        <v>1</v>
+      </c>
+      <c r="V65" t="n">
+        <v>0.244047619047619</v>
+      </c>
+      <c r="W65" t="n">
+        <v>0.2888888888888889</v>
+      </c>
+      <c r="X65" t="n">
+        <v>2.251542681017716</v>
+      </c>
+      <c r="Y65" t="n">
+        <v>1.967513941783161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25">
+      <c r="A66" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C66" t="s">
+        <v>72</v>
+      </c>
+      <c r="D66" t="s">
+        <v>28</v>
+      </c>
+      <c r="E66" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" t="s">
+        <v>39</v>
+      </c>
+      <c r="H66" t="s">
+        <v>32</v>
+      </c>
+      <c r="I66" t="s">
+        <v>33</v>
+      </c>
+      <c r="J66" t="s">
+        <v>118</v>
+      </c>
+      <c r="K66" t="s">
+        <v>35</v>
+      </c>
+      <c r="L66" t="s">
+        <v>29</v>
+      </c>
+      <c r="M66" t="s">
+        <v>74</v>
+      </c>
+      <c r="N66" t="n">
+        <v>2</v>
+      </c>
+      <c r="O66" t="n">
+        <v>0.06184496233860651</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0.1136452208624946</v>
+      </c>
+      <c r="Q66" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+      <c r="R66" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="S66" t="n">
+        <v>1.827914068349451</v>
+      </c>
+      <c r="T66" t="n">
+        <v>2.077391526784384</v>
+      </c>
+      <c r="U66" t="n">
+        <v>2</v>
+      </c>
+      <c r="V66" t="n">
+        <v>0.3571428571428572</v>
+      </c>
+      <c r="W66" t="n">
+        <v>0.2844444444444444</v>
+      </c>
+      <c r="X66" t="n">
+        <v>1.827914068349451</v>
+      </c>
+      <c r="Y66" t="n">
+        <v>2.077391526784384</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25">
+      <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D67" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" t="s">
+        <v>39</v>
+      </c>
+      <c r="H67" t="s">
+        <v>32</v>
+      </c>
+      <c r="I67" t="s">
+        <v>33</v>
+      </c>
+      <c r="J67" t="s">
+        <v>118</v>
+      </c>
+      <c r="K67" t="s">
+        <v>35</v>
+      </c>
+      <c r="L67" t="s">
+        <v>29</v>
+      </c>
+      <c r="M67" t="s">
+        <v>74</v>
+      </c>
+      <c r="S67" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25">
+      <c r="A68" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" t="s">
+        <v>71</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+      <c r="D68" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G68" t="s">
+        <v>39</v>
+      </c>
+      <c r="H68" t="s">
+        <v>32</v>
+      </c>
+      <c r="I68" t="s">
+        <v>33</v>
+      </c>
+      <c r="J68" t="s">
+        <v>118</v>
+      </c>
+      <c r="K68" t="s">
+        <v>35</v>
+      </c>
+      <c r="L68" t="s">
+        <v>29</v>
+      </c>
+      <c r="M68" t="s">
+        <v>74</v>
+      </c>
+      <c r="S68" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:25">
+      <c r="A69" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" t="s">
+        <v>71</v>
+      </c>
+      <c r="C69" t="s">
+        <v>72</v>
+      </c>
+      <c r="D69" t="s">
+        <v>28</v>
+      </c>
+      <c r="E69" t="s">
+        <v>29</v>
+      </c>
+      <c r="F69" t="s">
+        <v>30</v>
+      </c>
+      <c r="G69" t="s">
+        <v>39</v>
+      </c>
+      <c r="H69" t="s">
+        <v>32</v>
+      </c>
+      <c r="I69" t="s">
+        <v>33</v>
+      </c>
+      <c r="J69" t="s">
+        <v>118</v>
+      </c>
+      <c r="K69" t="s">
+        <v>35</v>
+      </c>
+      <c r="L69" t="s">
+        <v>29</v>
+      </c>
+      <c r="M69" t="s">
+        <v>74</v>
+      </c>
+      <c r="S69" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="70" spans="1:25">
+      <c r="A70" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" t="s">
+        <v>29</v>
+      </c>
+      <c r="F70" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" t="s">
+        <v>39</v>
+      </c>
+      <c r="H70" t="s">
+        <v>32</v>
+      </c>
+      <c r="I70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J70" t="s">
+        <v>118</v>
+      </c>
+      <c r="K70" t="s">
+        <v>35</v>
+      </c>
+      <c r="L70" t="s">
+        <v>29</v>
+      </c>
+      <c r="M70" t="s">
+        <v>74</v>
+      </c>
+      <c r="N70" t="n">
+        <v>2</v>
+      </c>
+      <c r="O70" t="n">
+        <v>0.05952280298584983</v>
+      </c>
+      <c r="P70" t="n">
+        <v>0.1204833539326986</v>
+      </c>
+      <c r="Q70" t="n">
+        <v>0.3690476190476191</v>
+      </c>
+      <c r="R70" t="n">
+        <v>0.2755555555555556</v>
+      </c>
+      <c r="S70" t="n">
+        <v>1.716516405813988</v>
+      </c>
+      <c r="T70" t="n">
+        <v>1.956186766816161</v>
+      </c>
+      <c r="U70" t="n">
+        <v>2</v>
+      </c>
+      <c r="V70" t="n">
+        <v>0.3690476190476191</v>
+      </c>
+      <c r="W70" t="n">
+        <v>0.2755555555555556</v>
+      </c>
+      <c r="X70" t="n">
+        <v>1.716516405813988</v>
+      </c>
+      <c r="Y70" t="n">
+        <v>1.956186766816161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:25">
+      <c r="A71" t="s">
+        <v>129</v>
+      </c>
+      <c r="B71" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" t="s">
+        <v>72</v>
+      </c>
+      <c r="D71" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" t="s">
+        <v>30</v>
+      </c>
+      <c r="G71" t="s">
+        <v>39</v>
+      </c>
+      <c r="H71" t="s">
+        <v>32</v>
+      </c>
+      <c r="I71" t="s">
+        <v>33</v>
+      </c>
+      <c r="J71" t="s">
+        <v>118</v>
+      </c>
+      <c r="K71" t="s">
+        <v>35</v>
+      </c>
+      <c r="L71" t="s">
+        <v>29</v>
+      </c>
+      <c r="M71" t="s">
+        <v>74</v>
+      </c>
+      <c r="N71" t="n">
+        <v>38</v>
+      </c>
+      <c r="O71" t="n">
+        <v>0.003310799798262971</v>
+      </c>
+      <c r="P71" t="n">
+        <v>0.1120523161358303</v>
+      </c>
+      <c r="Q71" t="n">
+        <v>0.9742063492063492</v>
+      </c>
+      <c r="R71" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="S71" t="n">
+        <v>0.3362963545672746</v>
+      </c>
+      <c r="T71" t="n">
+        <v>1.50406855635713</v>
+      </c>
+      <c r="U71" t="n">
+        <v>38</v>
+      </c>
+      <c r="V71" t="n">
+        <v>0.9742063492063492</v>
+      </c>
+      <c r="W71" t="n">
+        <v>0.3866666666666667</v>
+      </c>
+      <c r="X71" t="n">
+        <v>0.3362963545672746</v>
+      </c>
+      <c r="Y71" t="n">
+        <v>1.50406855635713</v>
+      </c>
+    </row>
+    <row r="72" spans="1:25">
+      <c r="A72" t="s">
+        <v>130</v>
+      </c>
+      <c r="B72" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" t="s">
+        <v>29</v>
+      </c>
+      <c r="F72" t="s">
+        <v>30</v>
+      </c>
+      <c r="G72" t="s">
+        <v>39</v>
+      </c>
+      <c r="H72" t="s">
+        <v>32</v>
+      </c>
+      <c r="I72" t="s">
+        <v>33</v>
+      </c>
+      <c r="J72" t="s">
+        <v>118</v>
+      </c>
+      <c r="K72" t="s">
+        <v>35</v>
+      </c>
+      <c r="L72" t="s">
+        <v>29</v>
+      </c>
+      <c r="M72" t="s">
+        <v>74</v>
+      </c>
+      <c r="N72" t="n">
+        <v>2</v>
+      </c>
+      <c r="O72" t="n">
+        <v>0.05038585904098693</v>
+      </c>
+      <c r="P72" t="n">
+        <v>0.08023414505852593</v>
+      </c>
+      <c r="Q72" t="n">
+        <v>0.3928571428571428</v>
+      </c>
+      <c r="R72" t="n">
+        <v>0.2933333333333333</v>
+      </c>
+      <c r="S72" t="n">
+        <v>1.56378915072861</v>
+      </c>
+      <c r="T72" t="n">
+        <v>1.717879830230017</v>
+      </c>
+      <c r="U72" t="n">
+        <v>2</v>
+      </c>
+      <c r="V72" t="n">
+        <v>0.3928571428571428</v>
+      </c>
+      <c r="W72" t="n">
+        <v>0.2933333333333333</v>
+      </c>
+      <c r="X72" t="n">
+        <v>1.56378915072861</v>
+      </c>
+      <c r="Y72" t="n">
+        <v>1.717879830230017</v>
+      </c>
+    </row>
+    <row r="73" spans="1:25">
+      <c r="A73" t="s">
+        <v>131</v>
+      </c>
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D73" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" t="s">
+        <v>39</v>
+      </c>
+      <c r="H73" t="s">
+        <v>32</v>
+      </c>
+      <c r="I73" t="s">
+        <v>33</v>
+      </c>
+      <c r="J73" t="s">
+        <v>118</v>
+      </c>
+      <c r="K73" t="s">
+        <v>35</v>
+      </c>
+      <c r="L73" t="s">
+        <v>29</v>
+      </c>
+      <c r="M73" t="s">
+        <v>74</v>
+      </c>
+      <c r="N73" t="n">
+        <v>2</v>
+      </c>
+      <c r="O73" t="n">
+        <v>0.05471803957507724</v>
+      </c>
+      <c r="P73" t="n">
+        <v>0.09047404792573717</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.3849206349206349</v>
+      </c>
+      <c r="R73" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="S73" t="n">
+        <v>1.786190412715338</v>
+      </c>
+      <c r="T73" t="n">
+        <v>1.907878402833891</v>
+      </c>
+      <c r="U73" t="n">
+        <v>2</v>
+      </c>
+      <c r="V73" t="n">
+        <v>0.3849206349206349</v>
+      </c>
+      <c r="W73" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="X73" t="n">
+        <v>1.786190412715338</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>1.907878402833891</v>
+      </c>
+    </row>
+    <row r="74" spans="1:25">
+      <c r="A74" t="s">
+        <v>132</v>
+      </c>
+      <c r="B74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" t="s">
+        <v>72</v>
+      </c>
+      <c r="D74" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" t="s">
+        <v>30</v>
+      </c>
+      <c r="G74" t="s">
+        <v>39</v>
+      </c>
+      <c r="H74" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" t="s">
+        <v>33</v>
+      </c>
+      <c r="J74" t="s">
+        <v>118</v>
+      </c>
+      <c r="K74" t="s">
+        <v>35</v>
+      </c>
+      <c r="L74" t="s">
+        <v>29</v>
+      </c>
+      <c r="M74" t="s">
+        <v>74</v>
+      </c>
+      <c r="N74" t="n">
+        <v>2</v>
+      </c>
+      <c r="O74" t="n">
+        <v>0.05069899298841991</v>
+      </c>
+      <c r="P74" t="n">
+        <v>0.0839737515979343</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0.3377777777777778</v>
+      </c>
+      <c r="S74" t="n">
+        <v>1.567274451507842</v>
+      </c>
+      <c r="T74" t="n">
+        <v>1.952775802116908</v>
+      </c>
+      <c r="U74" t="n">
+        <v>2</v>
+      </c>
+      <c r="V74" t="n">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="W74" t="n">
+        <v>0.3377777777777778</v>
+      </c>
+      <c r="X74" t="n">
+        <v>1.567274451507842</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>1.952775802116908</v>
+      </c>
+    </row>
+    <row r="75" spans="1:25">
+      <c r="A75" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" t="s">
+        <v>30</v>
+      </c>
+      <c r="G75" t="s">
+        <v>39</v>
+      </c>
+      <c r="H75" t="s">
+        <v>32</v>
+      </c>
+      <c r="I75" t="s">
+        <v>33</v>
+      </c>
+      <c r="J75" t="s">
+        <v>118</v>
+      </c>
+      <c r="K75" t="s">
+        <v>35</v>
+      </c>
+      <c r="L75" t="s">
+        <v>29</v>
+      </c>
+      <c r="M75" t="s">
+        <v>74</v>
+      </c>
+      <c r="N75" t="n">
+        <v>2</v>
+      </c>
+      <c r="O75" t="n">
+        <v>0.05583590564746705</v>
+      </c>
+      <c r="P75" t="n">
+        <v>0.08431223842832777</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.3998015873015873</v>
+      </c>
+      <c r="R75" t="n">
+        <v>0.2977777777777778</v>
+      </c>
+      <c r="S75" t="n">
+        <v>1.654119436773267</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1.916014381759989</v>
+      </c>
+      <c r="U75" t="n">
+        <v>2</v>
+      </c>
+      <c r="V75" t="n">
+        <v>0.3998015873015873</v>
+      </c>
+      <c r="W75" t="n">
+        <v>0.2977777777777778</v>
+      </c>
+      <c r="X75" t="n">
+        <v>1.654119436773267</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>1.916014381759989</v>
+      </c>
+    </row>
+    <row r="76" spans="1:25">
+      <c r="A76" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" t="s">
+        <v>72</v>
+      </c>
+      <c r="D76" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" t="s">
+        <v>29</v>
+      </c>
+      <c r="F76" t="s">
+        <v>30</v>
+      </c>
+      <c r="G76" t="s">
+        <v>39</v>
+      </c>
+      <c r="H76" t="s">
+        <v>32</v>
+      </c>
+      <c r="I76" t="s">
+        <v>33</v>
+      </c>
+      <c r="J76" t="s">
+        <v>118</v>
+      </c>
+      <c r="K76" t="s">
+        <v>35</v>
+      </c>
+      <c r="L76" t="s">
+        <v>29</v>
+      </c>
+      <c r="M76" t="s">
+        <v>74</v>
+      </c>
+      <c r="N76" t="n">
+        <v>2</v>
+      </c>
+      <c r="O76" t="n">
+        <v>0.0602247439443119</v>
+      </c>
+      <c r="P76" t="n">
+        <v>0.09726434787114462</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0.3809523809523809</v>
+      </c>
+      <c r="R76" t="n">
+        <v>0.2711111111111111</v>
+      </c>
+      <c r="S76" t="n">
+        <v>1.630257064158317</v>
+      </c>
+      <c r="T76" t="n">
+        <v>2.211083193570267</v>
+      </c>
+      <c r="U76" t="n">
+        <v>2</v>
+      </c>
+      <c r="V76" t="n">
+        <v>0.3809523809523809</v>
+      </c>
+      <c r="W76" t="n">
+        <v>0.2711111111111111</v>
+      </c>
+      <c r="X76" t="n">
+        <v>1.630257064158317</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>2.211083193570267</v>
+      </c>
+    </row>
+    <row r="77" spans="1:25">
+      <c r="A77" t="s">
+        <v>135</v>
+      </c>
+      <c r="B77" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" t="s">
+        <v>72</v>
+      </c>
+      <c r="D77" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" t="s">
+        <v>30</v>
+      </c>
+      <c r="G77" t="s">
+        <v>39</v>
+      </c>
+      <c r="H77" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" t="s">
+        <v>33</v>
+      </c>
+      <c r="J77" t="s">
+        <v>136</v>
+      </c>
+      <c r="K77" t="s">
+        <v>35</v>
+      </c>
+      <c r="L77" t="s">
+        <v>29</v>
+      </c>
+      <c r="M77" t="s">
+        <v>74</v>
+      </c>
+      <c r="S77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="78" spans="1:25">
+      <c r="A78" t="s">
+        <v>137</v>
+      </c>
+      <c r="B78" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="D78" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" t="s">
+        <v>29</v>
+      </c>
+      <c r="F78" t="s">
+        <v>30</v>
+      </c>
+      <c r="G78" t="s">
+        <v>39</v>
+      </c>
+      <c r="H78" t="s">
+        <v>32</v>
+      </c>
+      <c r="I78" t="s">
+        <v>33</v>
+      </c>
+      <c r="J78" t="s">
+        <v>136</v>
+      </c>
+      <c r="K78" t="s">
+        <v>35</v>
+      </c>
+      <c r="L78" t="s">
+        <v>29</v>
+      </c>
+      <c r="M78" t="s">
+        <v>74</v>
+      </c>
+      <c r="N78" t="n">
+        <v>2</v>
+      </c>
+      <c r="O78" t="n">
+        <v>0.03837354020770739</v>
+      </c>
+      <c r="P78" t="n">
+        <v>0.01966428215292925</v>
+      </c>
+      <c r="Q78" t="n">
+        <v>0.300081103000811</v>
+      </c>
+      <c r="R78" t="n">
+        <v>0.08110300081103</v>
+      </c>
+      <c r="S78" t="n">
+        <v>1.362217551845654</v>
+      </c>
+      <c r="T78" t="n">
+        <v>0.9285068112950217</v>
+      </c>
+      <c r="U78" t="n">
+        <v>2</v>
+      </c>
+      <c r="V78" t="n">
+        <v>0.300081103000811</v>
+      </c>
+      <c r="W78" t="n">
+        <v>0.08110300081103</v>
+      </c>
+      <c r="X78" t="n">
+        <v>1.362217551845654</v>
+      </c>
+      <c r="Y78" t="n">
+        <v>0.9285068112950217</v>
+      </c>
+    </row>
+    <row r="79" spans="1:25">
+      <c r="A79" t="s">
+        <v>138</v>
+      </c>
+      <c r="B79" t="s">
+        <v>71</v>
+      </c>
+      <c r="C79" t="s">
+        <v>72</v>
+      </c>
+      <c r="D79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" t="s">
+        <v>30</v>
+      </c>
+      <c r="G79" t="s">
+        <v>39</v>
+      </c>
+      <c r="H79" t="s">
+        <v>32</v>
+      </c>
+      <c r="I79" t="s">
+        <v>33</v>
+      </c>
+      <c r="J79" t="s">
+        <v>136</v>
+      </c>
+      <c r="K79" t="s">
+        <v>35</v>
+      </c>
+      <c r="L79" t="s">
+        <v>29</v>
+      </c>
+      <c r="M79" t="s">
+        <v>74</v>
+      </c>
+      <c r="N79" t="n">
+        <v>1</v>
+      </c>
+      <c r="O79" t="n">
+        <v>0.04628054416962784</v>
+      </c>
+      <c r="P79" t="n">
+        <v>0.01478456822431677</v>
+      </c>
+      <c r="Q79" t="n">
+        <v>0.2165450121654501</v>
+      </c>
+      <c r="R79" t="n">
+        <v>0.08921330089213302</v>
+      </c>
+      <c r="S79" t="n">
+        <v>1.799792724841541</v>
+      </c>
+      <c r="T79" t="n">
+        <v>0.8075073538492893</v>
+      </c>
+      <c r="U79" t="n">
+        <v>1</v>
+      </c>
+      <c r="V79" t="n">
+        <v>0.2165450121654501</v>
+      </c>
+      <c r="W79" t="n">
+        <v>0.08921330089213302</v>
+      </c>
+      <c r="X79" t="n">
+        <v>1.799792724841541</v>
+      </c>
+      <c r="Y79" t="n">
+        <v>0.8075073538492893</v>
+      </c>
+    </row>
+    <row r="80" spans="1:25">
+      <c r="A80" t="s">
+        <v>139</v>
+      </c>
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C80" t="s">
+        <v>72</v>
+      </c>
+      <c r="D80" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" t="s">
+        <v>30</v>
+      </c>
+      <c r="G80" t="s">
+        <v>39</v>
+      </c>
+      <c r="H80" t="s">
+        <v>32</v>
+      </c>
+      <c r="I80" t="s">
+        <v>33</v>
+      </c>
+      <c r="J80" t="s">
+        <v>136</v>
+      </c>
+      <c r="K80" t="s">
+        <v>35</v>
+      </c>
+      <c r="L80" t="s">
+        <v>29</v>
+      </c>
+      <c r="M80" t="s">
+        <v>74</v>
+      </c>
+      <c r="N80" t="n">
+        <v>2</v>
+      </c>
+      <c r="O80" t="n">
+        <v>0.03909223029406594</v>
+      </c>
+      <c r="P80" t="n">
+        <v>0.01627698277228263</v>
+      </c>
+      <c r="Q80" t="n">
+        <v>0.2984590429845904</v>
+      </c>
+      <c r="R80" t="n">
+        <v>0.06974858069748581</v>
+      </c>
+      <c r="S80" t="n">
+        <v>1.364596972963537</v>
+      </c>
+      <c r="T80" t="n">
+        <v>0.9509460862966862</v>
+      </c>
+      <c r="U80" t="n">
+        <v>2</v>
+      </c>
+      <c r="V80" t="n">
+        <v>0.2984590429845904</v>
+      </c>
+      <c r="W80" t="n">
+        <v>0.06974858069748581</v>
+      </c>
+      <c r="X80" t="n">
+        <v>1.364596972963537</v>
+      </c>
+      <c r="Y80" t="n">
+        <v>0.9509460862966862</v>
+      </c>
+    </row>
+    <row r="81" spans="1:25">
+      <c r="A81" t="s">
+        <v>140</v>
+      </c>
+      <c r="B81" t="s">
+        <v>71</v>
+      </c>
+      <c r="C81" t="s">
+        <v>72</v>
+      </c>
+      <c r="D81" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" t="s">
+        <v>29</v>
+      </c>
+      <c r="F81" t="s">
+        <v>30</v>
+      </c>
+      <c r="G81" t="s">
+        <v>39</v>
+      </c>
+      <c r="H81" t="s">
+        <v>32</v>
+      </c>
+      <c r="I81" t="s">
+        <v>33</v>
+      </c>
+      <c r="J81" t="s">
+        <v>136</v>
+      </c>
+      <c r="K81" t="s">
+        <v>35</v>
+      </c>
+      <c r="L81" t="s">
+        <v>29</v>
+      </c>
+      <c r="M81" t="s">
+        <v>74</v>
+      </c>
+      <c r="N81" t="n">
+        <v>1</v>
+      </c>
+      <c r="O81" t="n">
+        <v>0.048717105959067</v>
+      </c>
+      <c r="P81" t="n">
+        <v>0.01589492405708109</v>
+      </c>
+      <c r="Q81" t="n">
+        <v>0.1857258718572587</v>
+      </c>
+      <c r="R81" t="n">
+        <v>0.064882400648824</v>
+      </c>
+      <c r="S81" t="n">
+        <v>1.912735310121493</v>
+      </c>
+      <c r="T81" t="n">
+        <v>0.8717425753049757</v>
+      </c>
+      <c r="U81" t="n">
+        <v>1</v>
+      </c>
+      <c r="V81" t="n">
+        <v>0.1857258718572587</v>
+      </c>
+      <c r="W81" t="n">
+        <v>0.064882400648824</v>
+      </c>
+      <c r="X81" t="n">
+        <v>1.912735310121493</v>
+      </c>
+      <c r="Y81" t="n">
+        <v>0.8717425753049757</v>
+      </c>
+    </row>
     <row customHeight="1" ht="12.8" r="1048576" s="3" spans="1:25"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>

<commit_message>
New results with more detail
</commit_message>
<xml_diff>
--- a/logs.xlsx
+++ b/logs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
   <si>
     <t>Date</t>
   </si>
@@ -437,6 +437,54 @@
   </si>
   <si>
     <t>November08  19:16:50</t>
+  </si>
+  <si>
+    <t>November08  19:23:17</t>
+  </si>
+  <si>
+    <t>&lt;function exp_lr_scheduler at 0x7f07ec316ae8&gt;</t>
+  </si>
+  <si>
+    <t>November08  19:23:19</t>
+  </si>
+  <si>
+    <t>November08  19:26:51</t>
+  </si>
+  <si>
+    <t>November08  19:29:56</t>
+  </si>
+  <si>
+    <t>November08  19:35:46</t>
+  </si>
+  <si>
+    <t>November08  19:41:39</t>
+  </si>
+  <si>
+    <t>November08  19:47:31</t>
+  </si>
+  <si>
+    <t>November08  19:53:23</t>
+  </si>
+  <si>
+    <t>November08  19:59:12</t>
+  </si>
+  <si>
+    <t>November08  20:05:03</t>
+  </si>
+  <si>
+    <t>November08  20:10:56</t>
+  </si>
+  <si>
+    <t>November08  20:16:48</t>
+  </si>
+  <si>
+    <t>November08  20:22:45</t>
+  </si>
+  <si>
+    <t>November08  20:28:38</t>
+  </si>
+  <si>
+    <t>November08  20:34:32</t>
   </si>
 </sst>
 </file>
@@ -814,7 +862,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:Y81"/>
+  <dimension ref="A1:Y96"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A182" activeCellId="0" pane="topLeft" sqref="2:182"/>
@@ -6605,6 +6653,1128 @@
         <v>0.8717425753049757</v>
       </c>
     </row>
+    <row r="82" spans="1:25">
+      <c r="A82" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" t="s">
+        <v>71</v>
+      </c>
+      <c r="C82" t="s">
+        <v>72</v>
+      </c>
+      <c r="D82" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" t="s">
+        <v>30</v>
+      </c>
+      <c r="G82" t="s">
+        <v>39</v>
+      </c>
+      <c r="H82" t="s">
+        <v>32</v>
+      </c>
+      <c r="I82" t="s">
+        <v>33</v>
+      </c>
+      <c r="J82" t="s">
+        <v>142</v>
+      </c>
+      <c r="K82" t="s">
+        <v>35</v>
+      </c>
+      <c r="L82" t="s">
+        <v>29</v>
+      </c>
+      <c r="M82" t="s">
+        <v>74</v>
+      </c>
+      <c r="S82" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="1:25">
+      <c r="A83" t="s">
+        <v>143</v>
+      </c>
+      <c r="B83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C83" t="s">
+        <v>72</v>
+      </c>
+      <c r="D83" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" t="s">
+        <v>30</v>
+      </c>
+      <c r="G83" t="s">
+        <v>39</v>
+      </c>
+      <c r="H83" t="s">
+        <v>32</v>
+      </c>
+      <c r="I83" t="s">
+        <v>33</v>
+      </c>
+      <c r="J83" t="s">
+        <v>142</v>
+      </c>
+      <c r="K83" t="s">
+        <v>35</v>
+      </c>
+      <c r="L83" t="s">
+        <v>29</v>
+      </c>
+      <c r="M83" t="s">
+        <v>74</v>
+      </c>
+      <c r="N83" t="n">
+        <v>5</v>
+      </c>
+      <c r="O83" t="n">
+        <v>0.04334113671348429</v>
+      </c>
+      <c r="P83" t="n">
+        <v>0.0281702742790267</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>0.5352798053527981</v>
+      </c>
+      <c r="R83" t="n">
+        <v>0.6747769667477697</v>
+      </c>
+      <c r="S83" t="n">
+        <v>1.388751006943395</v>
+      </c>
+      <c r="T83" t="n">
+        <v>1.111030005150121</v>
+      </c>
+      <c r="U83" t="n">
+        <v>5</v>
+      </c>
+      <c r="V83" t="n">
+        <v>0.5352798053527981</v>
+      </c>
+      <c r="W83" t="n">
+        <v>0.6747769667477697</v>
+      </c>
+      <c r="X83" t="n">
+        <v>1.388751006943395</v>
+      </c>
+      <c r="Y83" t="n">
+        <v>1.111030005150121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:25">
+      <c r="A84" t="s">
+        <v>144</v>
+      </c>
+      <c r="B84" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" t="s">
+        <v>72</v>
+      </c>
+      <c r="D84" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" t="s">
+        <v>30</v>
+      </c>
+      <c r="G84" t="s">
+        <v>39</v>
+      </c>
+      <c r="H84" t="s">
+        <v>32</v>
+      </c>
+      <c r="I84" t="s">
+        <v>33</v>
+      </c>
+      <c r="J84" t="s">
+        <v>142</v>
+      </c>
+      <c r="K84" t="s">
+        <v>35</v>
+      </c>
+      <c r="L84" t="s">
+        <v>29</v>
+      </c>
+      <c r="M84" t="s">
+        <v>74</v>
+      </c>
+      <c r="N84" t="n">
+        <v>2</v>
+      </c>
+      <c r="O84" t="n">
+        <v>0.0419952683785246</v>
+      </c>
+      <c r="P84" t="n">
+        <v>0.01750046590045518</v>
+      </c>
+      <c r="Q84" t="n">
+        <v>0.3098134630981346</v>
+      </c>
+      <c r="R84" t="n">
+        <v>0.07137064071370641</v>
+      </c>
+      <c r="S84" t="n">
+        <v>1.379081349673997</v>
+      </c>
+      <c r="T84" t="n">
+        <v>0.8054961244402359</v>
+      </c>
+      <c r="U84" t="n">
+        <v>2</v>
+      </c>
+      <c r="V84" t="n">
+        <v>0.3098134630981346</v>
+      </c>
+      <c r="W84" t="n">
+        <v>0.07137064071370641</v>
+      </c>
+      <c r="X84" t="n">
+        <v>1.379081349673997</v>
+      </c>
+      <c r="Y84" t="n">
+        <v>0.8054961244402359</v>
+      </c>
+    </row>
+    <row r="85" spans="1:25">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" t="s">
+        <v>71</v>
+      </c>
+      <c r="C85" t="s">
+        <v>72</v>
+      </c>
+      <c r="D85" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" t="s">
+        <v>30</v>
+      </c>
+      <c r="G85" t="s">
+        <v>39</v>
+      </c>
+      <c r="H85" t="s">
+        <v>32</v>
+      </c>
+      <c r="I85" t="s">
+        <v>33</v>
+      </c>
+      <c r="J85" t="s">
+        <v>142</v>
+      </c>
+      <c r="K85" t="s">
+        <v>35</v>
+      </c>
+      <c r="L85" t="s">
+        <v>29</v>
+      </c>
+      <c r="M85" t="s">
+        <v>74</v>
+      </c>
+      <c r="N85" t="n">
+        <v>20</v>
+      </c>
+      <c r="O85" t="n">
+        <v>0.002690032043885359</v>
+      </c>
+      <c r="P85" t="n">
+        <v>0.07745679709818457</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>0.9816017316017316</v>
+      </c>
+      <c r="R85" t="n">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="S85" t="n">
+        <v>0.2326210525996177</v>
+      </c>
+      <c r="T85" t="n">
+        <v>1.421084275995101</v>
+      </c>
+      <c r="U85" t="n">
+        <v>20</v>
+      </c>
+      <c r="V85" t="n">
+        <v>0.9816017316017316</v>
+      </c>
+      <c r="W85" t="n">
+        <v>0.4090909090909091</v>
+      </c>
+      <c r="X85" t="n">
+        <v>0.2326210525996177</v>
+      </c>
+      <c r="Y85" t="n">
+        <v>1.421084275995101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:25">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C86" t="s">
+        <v>72</v>
+      </c>
+      <c r="D86" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" t="s">
+        <v>30</v>
+      </c>
+      <c r="G86" t="s">
+        <v>39</v>
+      </c>
+      <c r="H86" t="s">
+        <v>32</v>
+      </c>
+      <c r="I86" t="s">
+        <v>33</v>
+      </c>
+      <c r="J86" t="s">
+        <v>142</v>
+      </c>
+      <c r="K86" t="s">
+        <v>35</v>
+      </c>
+      <c r="L86" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" t="s">
+        <v>74</v>
+      </c>
+      <c r="N86" t="n">
+        <v>26</v>
+      </c>
+      <c r="O86" t="n">
+        <v>0.00232736115622056</v>
+      </c>
+      <c r="P86" t="n">
+        <v>0.07711041399410792</v>
+      </c>
+      <c r="Q86" t="n">
+        <v>0.9816017316017316</v>
+      </c>
+      <c r="R86" t="n">
+        <v>0.3863636363636364</v>
+      </c>
+      <c r="S86" t="n">
+        <v>0.3068482428756015</v>
+      </c>
+      <c r="T86" t="n">
+        <v>1.403844443226963</v>
+      </c>
+      <c r="U86" t="n">
+        <v>26</v>
+      </c>
+      <c r="V86" t="n">
+        <v>0.9816017316017316</v>
+      </c>
+      <c r="W86" t="n">
+        <v>0.3863636363636364</v>
+      </c>
+      <c r="X86" t="n">
+        <v>0.3068482428756015</v>
+      </c>
+      <c r="Y86" t="n">
+        <v>1.403844443226963</v>
+      </c>
+    </row>
+    <row r="87" spans="1:25">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C87" t="s">
+        <v>72</v>
+      </c>
+      <c r="D87" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" t="s">
+        <v>29</v>
+      </c>
+      <c r="F87" t="s">
+        <v>30</v>
+      </c>
+      <c r="G87" t="s">
+        <v>39</v>
+      </c>
+      <c r="H87" t="s">
+        <v>32</v>
+      </c>
+      <c r="I87" t="s">
+        <v>33</v>
+      </c>
+      <c r="J87" t="s">
+        <v>142</v>
+      </c>
+      <c r="K87" t="s">
+        <v>35</v>
+      </c>
+      <c r="L87" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" t="s">
+        <v>74</v>
+      </c>
+      <c r="N87" t="n">
+        <v>24</v>
+      </c>
+      <c r="O87" t="n">
+        <v>0.003207404706707764</v>
+      </c>
+      <c r="P87" t="n">
+        <v>0.08552800796248695</v>
+      </c>
+      <c r="Q87" t="n">
+        <v>0.9761904761904762</v>
+      </c>
+      <c r="R87" t="n">
+        <v>0.3766233766233766</v>
+      </c>
+      <c r="S87" t="n">
+        <v>0.3512500866571044</v>
+      </c>
+      <c r="T87" t="n">
+        <v>1.536355951721349</v>
+      </c>
+      <c r="U87" t="n">
+        <v>24</v>
+      </c>
+      <c r="V87" t="n">
+        <v>0.9761904761904762</v>
+      </c>
+      <c r="W87" t="n">
+        <v>0.3766233766233766</v>
+      </c>
+      <c r="X87" t="n">
+        <v>0.3512500866571044</v>
+      </c>
+      <c r="Y87" t="n">
+        <v>1.536355951721349</v>
+      </c>
+    </row>
+    <row r="88" spans="1:25">
+      <c r="A88" t="s">
+        <v>148</v>
+      </c>
+      <c r="B88" t="s">
+        <v>71</v>
+      </c>
+      <c r="C88" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" t="s">
+        <v>29</v>
+      </c>
+      <c r="F88" t="s">
+        <v>30</v>
+      </c>
+      <c r="G88" t="s">
+        <v>39</v>
+      </c>
+      <c r="H88" t="s">
+        <v>32</v>
+      </c>
+      <c r="I88" t="s">
+        <v>33</v>
+      </c>
+      <c r="J88" t="s">
+        <v>142</v>
+      </c>
+      <c r="K88" t="s">
+        <v>35</v>
+      </c>
+      <c r="L88" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" t="s">
+        <v>74</v>
+      </c>
+      <c r="N88" t="n">
+        <v>22</v>
+      </c>
+      <c r="O88" t="n">
+        <v>0.002484592242222844</v>
+      </c>
+      <c r="P88" t="n">
+        <v>0.07642197802469328</v>
+      </c>
+      <c r="Q88" t="n">
+        <v>0.974025974025974</v>
+      </c>
+      <c r="R88" t="n">
+        <v>0.3993506493506493</v>
+      </c>
+      <c r="S88" t="n">
+        <v>0.3434608681718603</v>
+      </c>
+      <c r="T88" t="n">
+        <v>1.456066574758816</v>
+      </c>
+      <c r="U88" t="n">
+        <v>22</v>
+      </c>
+      <c r="V88" t="n">
+        <v>0.974025974025974</v>
+      </c>
+      <c r="W88" t="n">
+        <v>0.3993506493506493</v>
+      </c>
+      <c r="X88" t="n">
+        <v>0.3434608681718603</v>
+      </c>
+      <c r="Y88" t="n">
+        <v>1.456066574758816</v>
+      </c>
+    </row>
+    <row r="89" spans="1:25">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>71</v>
+      </c>
+      <c r="C89" t="s">
+        <v>72</v>
+      </c>
+      <c r="D89" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" t="s">
+        <v>30</v>
+      </c>
+      <c r="G89" t="s">
+        <v>31</v>
+      </c>
+      <c r="H89" t="s">
+        <v>32</v>
+      </c>
+      <c r="I89" t="s">
+        <v>33</v>
+      </c>
+      <c r="J89" t="s">
+        <v>142</v>
+      </c>
+      <c r="K89" t="s">
+        <v>35</v>
+      </c>
+      <c r="L89" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" t="s">
+        <v>74</v>
+      </c>
+      <c r="N89" t="n">
+        <v>14</v>
+      </c>
+      <c r="O89" t="n">
+        <v>0.00454240246349341</v>
+      </c>
+      <c r="P89" t="n">
+        <v>0.01250092022411235</v>
+      </c>
+      <c r="Q89" t="n">
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="R89" t="n">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="S89" t="n">
+        <v>0.719246840323972</v>
+      </c>
+      <c r="T89" t="n">
+        <v>1.237928726731686</v>
+      </c>
+      <c r="U89" t="n">
+        <v>14</v>
+      </c>
+      <c r="V89" t="n">
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="W89" t="n">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="X89" t="n">
+        <v>0.719246840323972</v>
+      </c>
+      <c r="Y89" t="n">
+        <v>1.237928726731686</v>
+      </c>
+    </row>
+    <row r="90" spans="1:25">
+      <c r="A90" t="s">
+        <v>150</v>
+      </c>
+      <c r="B90" t="s">
+        <v>71</v>
+      </c>
+      <c r="C90" t="s">
+        <v>72</v>
+      </c>
+      <c r="D90" t="s">
+        <v>28</v>
+      </c>
+      <c r="E90" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" t="s">
+        <v>30</v>
+      </c>
+      <c r="G90" t="s">
+        <v>31</v>
+      </c>
+      <c r="H90" t="s">
+        <v>32</v>
+      </c>
+      <c r="I90" t="s">
+        <v>33</v>
+      </c>
+      <c r="J90" t="s">
+        <v>142</v>
+      </c>
+      <c r="K90" t="s">
+        <v>35</v>
+      </c>
+      <c r="L90" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" t="s">
+        <v>74</v>
+      </c>
+      <c r="N90" t="n">
+        <v>7</v>
+      </c>
+      <c r="O90" t="n">
+        <v>0.007189551182897576</v>
+      </c>
+      <c r="P90" t="n">
+        <v>0.01224703931963289</v>
+      </c>
+      <c r="Q90" t="n">
+        <v>0.4675324675324675</v>
+      </c>
+      <c r="R90" t="n">
+        <v>0.3311688311688312</v>
+      </c>
+      <c r="S90" t="n">
+        <v>0.8765832923335172</v>
+      </c>
+      <c r="T90" t="n">
+        <v>1.289316742440608</v>
+      </c>
+      <c r="U90" t="n">
+        <v>7</v>
+      </c>
+      <c r="V90" t="n">
+        <v>0.4675324675324675</v>
+      </c>
+      <c r="W90" t="n">
+        <v>0.3311688311688312</v>
+      </c>
+      <c r="X90" t="n">
+        <v>0.8765832923335172</v>
+      </c>
+      <c r="Y90" t="n">
+        <v>1.289316742440608</v>
+      </c>
+    </row>
+    <row r="91" spans="1:25">
+      <c r="A91" t="s">
+        <v>151</v>
+      </c>
+      <c r="B91" t="s">
+        <v>71</v>
+      </c>
+      <c r="C91" t="s">
+        <v>72</v>
+      </c>
+      <c r="D91" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" t="s">
+        <v>29</v>
+      </c>
+      <c r="F91" t="s">
+        <v>30</v>
+      </c>
+      <c r="G91" t="s">
+        <v>31</v>
+      </c>
+      <c r="H91" t="s">
+        <v>32</v>
+      </c>
+      <c r="I91" t="s">
+        <v>33</v>
+      </c>
+      <c r="J91" t="s">
+        <v>142</v>
+      </c>
+      <c r="K91" t="s">
+        <v>35</v>
+      </c>
+      <c r="L91" t="s">
+        <v>29</v>
+      </c>
+      <c r="M91" t="s">
+        <v>74</v>
+      </c>
+      <c r="N91" t="n">
+        <v>19</v>
+      </c>
+      <c r="O91" t="n">
+        <v>0.003655296125453272</v>
+      </c>
+      <c r="P91" t="n">
+        <v>0.01348998949125216</v>
+      </c>
+      <c r="Q91" t="n">
+        <v>0.6006493506493507</v>
+      </c>
+      <c r="R91" t="n">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="S91" t="n">
+        <v>0.6546536707079771</v>
+      </c>
+      <c r="T91" t="n">
+        <v>1.310546629285836</v>
+      </c>
+      <c r="U91" t="n">
+        <v>19</v>
+      </c>
+      <c r="V91" t="n">
+        <v>0.6006493506493507</v>
+      </c>
+      <c r="W91" t="n">
+        <v>0.3636363636363636</v>
+      </c>
+      <c r="X91" t="n">
+        <v>0.6546536707079771</v>
+      </c>
+      <c r="Y91" t="n">
+        <v>1.310546629285836</v>
+      </c>
+    </row>
+    <row r="92" spans="1:25">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+      <c r="B92" t="s">
+        <v>71</v>
+      </c>
+      <c r="C92" t="s">
+        <v>72</v>
+      </c>
+      <c r="D92" t="s">
+        <v>28</v>
+      </c>
+      <c r="E92" t="s">
+        <v>29</v>
+      </c>
+      <c r="F92" t="s">
+        <v>30</v>
+      </c>
+      <c r="G92" t="s">
+        <v>31</v>
+      </c>
+      <c r="H92" t="s">
+        <v>32</v>
+      </c>
+      <c r="I92" t="s">
+        <v>33</v>
+      </c>
+      <c r="J92" t="s">
+        <v>142</v>
+      </c>
+      <c r="K92" t="s">
+        <v>35</v>
+      </c>
+      <c r="L92" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" t="s">
+        <v>74</v>
+      </c>
+      <c r="N92" t="n">
+        <v>16</v>
+      </c>
+      <c r="O92" t="n">
+        <v>0.00432416656381124</v>
+      </c>
+      <c r="P92" t="n">
+        <v>0.01360972293398597</v>
+      </c>
+      <c r="Q92" t="n">
+        <v>0.5573593073593074</v>
+      </c>
+      <c r="R92" t="n">
+        <v>0.3733766233766234</v>
+      </c>
+      <c r="S92" t="n">
+        <v>0.7222499717168716</v>
+      </c>
+      <c r="T92" t="n">
+        <v>1.258735708723473</v>
+      </c>
+      <c r="U92" t="n">
+        <v>16</v>
+      </c>
+      <c r="V92" t="n">
+        <v>0.5573593073593074</v>
+      </c>
+      <c r="W92" t="n">
+        <v>0.3733766233766234</v>
+      </c>
+      <c r="X92" t="n">
+        <v>0.7222499717168716</v>
+      </c>
+      <c r="Y92" t="n">
+        <v>1.258735708723473</v>
+      </c>
+    </row>
+    <row r="93" spans="1:25">
+      <c r="A93" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" t="s">
+        <v>71</v>
+      </c>
+      <c r="C93" t="s">
+        <v>72</v>
+      </c>
+      <c r="D93" t="s">
+        <v>28</v>
+      </c>
+      <c r="E93" t="s">
+        <v>29</v>
+      </c>
+      <c r="F93" t="s">
+        <v>30</v>
+      </c>
+      <c r="G93" t="s">
+        <v>99</v>
+      </c>
+      <c r="H93" t="s">
+        <v>32</v>
+      </c>
+      <c r="I93" t="s">
+        <v>33</v>
+      </c>
+      <c r="J93" t="s">
+        <v>142</v>
+      </c>
+      <c r="K93" t="s">
+        <v>35</v>
+      </c>
+      <c r="L93" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" t="s">
+        <v>74</v>
+      </c>
+      <c r="N93" t="n">
+        <v>19</v>
+      </c>
+      <c r="O93" t="n">
+        <v>0.004559562214976782</v>
+      </c>
+      <c r="P93" t="n">
+        <v>0.01790383312996332</v>
+      </c>
+      <c r="Q93" t="n">
+        <v>0.8885281385281385</v>
+      </c>
+      <c r="R93" t="n">
+        <v>0.4318181818181818</v>
+      </c>
+      <c r="S93" t="n">
+        <v>0.5243012253388074</v>
+      </c>
+      <c r="T93" t="n">
+        <v>1.306825239958353</v>
+      </c>
+      <c r="U93" t="n">
+        <v>19</v>
+      </c>
+      <c r="V93" t="n">
+        <v>0.8885281385281385</v>
+      </c>
+      <c r="W93" t="n">
+        <v>0.4318181818181818</v>
+      </c>
+      <c r="X93" t="n">
+        <v>0.5243012253388074</v>
+      </c>
+      <c r="Y93" t="n">
+        <v>1.306825239958353</v>
+      </c>
+    </row>
+    <row r="94" spans="1:25">
+      <c r="A94" t="s">
+        <v>154</v>
+      </c>
+      <c r="B94" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" t="s">
+        <v>72</v>
+      </c>
+      <c r="D94" t="s">
+        <v>28</v>
+      </c>
+      <c r="E94" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" t="s">
+        <v>30</v>
+      </c>
+      <c r="G94" t="s">
+        <v>99</v>
+      </c>
+      <c r="H94" t="s">
+        <v>32</v>
+      </c>
+      <c r="I94" t="s">
+        <v>33</v>
+      </c>
+      <c r="J94" t="s">
+        <v>142</v>
+      </c>
+      <c r="K94" t="s">
+        <v>35</v>
+      </c>
+      <c r="L94" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" t="s">
+        <v>74</v>
+      </c>
+      <c r="N94" t="n">
+        <v>30</v>
+      </c>
+      <c r="O94" t="n">
+        <v>0.0036955579341232</v>
+      </c>
+      <c r="P94" t="n">
+        <v>0.01761063381836012</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>0.908008658008658</v>
+      </c>
+      <c r="R94" t="n">
+        <v>0.4448051948051948</v>
+      </c>
+      <c r="S94" t="n">
+        <v>0.3678061789603123</v>
+      </c>
+      <c r="T94" t="n">
+        <v>1.1870513506546</v>
+      </c>
+      <c r="U94" t="n">
+        <v>30</v>
+      </c>
+      <c r="V94" t="n">
+        <v>0.908008658008658</v>
+      </c>
+      <c r="W94" t="n">
+        <v>0.4448051948051948</v>
+      </c>
+      <c r="X94" t="n">
+        <v>0.3678061789603123</v>
+      </c>
+      <c r="Y94" t="n">
+        <v>1.1870513506546</v>
+      </c>
+    </row>
+    <row r="95" spans="1:25">
+      <c r="A95" t="s">
+        <v>155</v>
+      </c>
+      <c r="B95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C95" t="s">
+        <v>72</v>
+      </c>
+      <c r="D95" t="s">
+        <v>28</v>
+      </c>
+      <c r="E95" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" t="s">
+        <v>30</v>
+      </c>
+      <c r="G95" t="s">
+        <v>99</v>
+      </c>
+      <c r="H95" t="s">
+        <v>32</v>
+      </c>
+      <c r="I95" t="s">
+        <v>33</v>
+      </c>
+      <c r="J95" t="s">
+        <v>142</v>
+      </c>
+      <c r="K95" t="s">
+        <v>35</v>
+      </c>
+      <c r="L95" t="s">
+        <v>29</v>
+      </c>
+      <c r="M95" t="s">
+        <v>74</v>
+      </c>
+      <c r="N95" t="n">
+        <v>14</v>
+      </c>
+      <c r="O95" t="n">
+        <v>0.004371386480989394</v>
+      </c>
+      <c r="P95" t="n">
+        <v>0.01904632364000593</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>0.8766233766233766</v>
+      </c>
+      <c r="R95" t="n">
+        <v>0.4318181818181818</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0.4912657034049816</v>
+      </c>
+      <c r="T95" t="n">
+        <v>1.28427047359606</v>
+      </c>
+      <c r="U95" t="n">
+        <v>14</v>
+      </c>
+      <c r="V95" t="n">
+        <v>0.8766233766233766</v>
+      </c>
+      <c r="W95" t="n">
+        <v>0.4318181818181818</v>
+      </c>
+      <c r="X95" t="n">
+        <v>0.4912657034049816</v>
+      </c>
+      <c r="Y95" t="n">
+        <v>1.28427047359606</v>
+      </c>
+    </row>
+    <row r="96" spans="1:25">
+      <c r="A96" t="s">
+        <v>156</v>
+      </c>
+      <c r="B96" t="s">
+        <v>71</v>
+      </c>
+      <c r="C96" t="s">
+        <v>72</v>
+      </c>
+      <c r="D96" t="s">
+        <v>28</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" t="s">
+        <v>30</v>
+      </c>
+      <c r="G96" t="s">
+        <v>99</v>
+      </c>
+      <c r="H96" t="s">
+        <v>32</v>
+      </c>
+      <c r="I96" t="s">
+        <v>33</v>
+      </c>
+      <c r="J96" t="s">
+        <v>142</v>
+      </c>
+      <c r="K96" t="s">
+        <v>35</v>
+      </c>
+      <c r="L96" t="s">
+        <v>29</v>
+      </c>
+      <c r="M96" t="s">
+        <v>74</v>
+      </c>
+      <c r="N96" t="n">
+        <v>25</v>
+      </c>
+      <c r="O96" t="n">
+        <v>0.003952494100768329</v>
+      </c>
+      <c r="P96" t="n">
+        <v>0.02005540086077405</v>
+      </c>
+      <c r="Q96" t="n">
+        <v>0.8852813852813853</v>
+      </c>
+      <c r="R96" t="n">
+        <v>0.3863636363636364</v>
+      </c>
+      <c r="S96" t="n">
+        <v>0.4301917422091399</v>
+      </c>
+      <c r="T96" t="n">
+        <v>1.245772070624499</v>
+      </c>
+      <c r="U96" t="n">
+        <v>25</v>
+      </c>
+      <c r="V96" t="n">
+        <v>0.8852813852813853</v>
+      </c>
+      <c r="W96" t="n">
+        <v>0.3863636363636364</v>
+      </c>
+      <c r="X96" t="n">
+        <v>0.4301917422091399</v>
+      </c>
+      <c r="Y96" t="n">
+        <v>1.245772070624499</v>
+      </c>
+    </row>
     <row customHeight="1" ht="12.8" r="1048576" s="3" spans="1:25"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>

</xml_diff>